<commit_message>
update data and graph
</commit_message>
<xml_diff>
--- a/rawdata/01 EGAT_EV_เตรียมข้อมูลประชุม_Sep2023.xlsx
+++ b/rawdata/01 EGAT_EV_เตรียมข้อมูลประชุม_Sep2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rstudio\thailandVehicleAnalysis\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBF19CC-C2B9-44BA-8B80-228A05B3CDF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A67D12-2671-4FE2-8A3A-190BBAE9068D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{EDD8F08D-6CA6-4516-B97F-8A475C3F3159}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="2" activeTab="2" xr2:uid="{EDD8F08D-6CA6-4516-B97F-8A475C3F3159}"/>
   </bookViews>
   <sheets>
     <sheet name="M2_Ques_Sep22" sheetId="3" r:id="rId1"/>
@@ -7298,7 +7298,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>549363</xdr:colOff>
+      <xdr:colOff>513504</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>4705</xdr:rowOff>
     </xdr:to>
@@ -7342,7 +7342,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>470647</xdr:colOff>
+      <xdr:colOff>434788</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>89648</xdr:rowOff>
     </xdr:to>
@@ -7372,13 +7372,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>506504</xdr:colOff>
+      <xdr:colOff>470645</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>134470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>170330</xdr:colOff>
+      <xdr:colOff>134471</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>80682</xdr:rowOff>
     </xdr:to>
@@ -7408,13 +7408,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>242048</xdr:colOff>
+      <xdr:colOff>206189</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>125505</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>125507</xdr:colOff>
+      <xdr:colOff>89648</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>71717</xdr:rowOff>
     </xdr:to>
@@ -7444,13 +7444,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>179296</xdr:colOff>
+      <xdr:colOff>143437</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>116541</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>98612</xdr:colOff>
+      <xdr:colOff>62753</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>62753</xdr:rowOff>
     </xdr:to>
@@ -8647,7 +8647,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-      <selection pane="bottomRight" activeCell="R30" sqref="R30"/>
+      <selection pane="bottomRight" activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -8660,7 +8660,7 @@
     <col min="12" max="12" width="14.19921875" style="31" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" style="31" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="8.69921875" style="32"/>
-    <col min="16" max="16" width="7.5" style="32" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" style="32" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.8984375" style="32" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="32" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.8984375" style="32" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
update EV unit of September 2023. EV increases from 90,000 units in Aug2023 to 97,400 units in Sep2023.
</commit_message>
<xml_diff>
--- a/rawdata/01 EGAT_EV_เตรียมข้อมูลประชุม_Sep2023.xlsx
+++ b/rawdata/01 EGAT_EV_เตรียมข้อมูลประชุม_Sep2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rstudio\thailandVehicleAnalysis\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A67D12-2671-4FE2-8A3A-190BBAE9068D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F617BE2B-BA3A-418E-A4F7-7E0C782EE485}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="2" activeTab="2" xr2:uid="{EDD8F08D-6CA6-4516-B97F-8A475C3F3159}"/>
   </bookViews>
@@ -1003,7 +1003,7 @@
     <t>ส่วนเพิ่ม BEV/รถทุกเชื้อเพลิง</t>
   </si>
   <si>
-    <t>31 สิงหาคม 2566</t>
+    <t>31 กันยายน 2566</t>
   </si>
 </sst>
 </file>
@@ -1011,11 +1011,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="187" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="188" formatCode="B1mmm\-yy"/>
-    <numFmt numFmtId="189" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="190" formatCode="[$-107041E]d\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="191" formatCode="0.0%"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="187" formatCode="B1mmm\-yy"/>
+    <numFmt numFmtId="188" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="189" formatCode="[$-107041E]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="190" formatCode="0.0%"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -1308,7 +1308,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -1331,7 +1331,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="188" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="187" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1343,36 +1343,36 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="4" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="4" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="191" fontId="5" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="191" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="190" fontId="5" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="190" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1382,7 +1382,7 @@
     <xf numFmtId="1" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="190" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="189" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1394,12 +1394,12 @@
     <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="190" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="189" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="7" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="7" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1417,7 +1417,7 @@
     <xf numFmtId="1" fontId="7" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="190" fontId="7" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="189" fontId="7" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1448,10 +1448,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="188" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="188" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1460,25 +1460,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="189" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="188" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="190" fontId="7" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="189" fontId="7" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="190" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="188" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="190" fontId="7" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="189" fontId="7" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="191" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="190" fontId="7" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="7" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1577,7 +1577,7 @@
                   <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31 สิงหาคม 2566</c:v>
+                  <c:v>31 กันยายน 2566</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1613,7 +1613,7 @@
                   <c:v>13732</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>57049</c:v>
+                  <c:v>63880</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1681,7 +1681,7 @@
                   <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31 สิงหาคม 2566</c:v>
+                  <c:v>31 กันยายน 2566</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1717,7 +1717,7 @@
                   <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>151</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1785,7 +1785,7 @@
                   <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31 สิงหาคม 2566</c:v>
+                  <c:v>31 กันยายน 2566</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1821,7 +1821,7 @@
                   <c:v>17038</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31114</c:v>
+                  <c:v>33051</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1889,7 +1889,7 @@
                   <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31 สิงหาคม 2566</c:v>
+                  <c:v>31 กันยายน 2566</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1925,7 +1925,7 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>251</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1993,7 +1993,7 @@
                   <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31 สิงหาคม 2566</c:v>
+                  <c:v>31 กันยายน 2566</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2029,7 +2029,7 @@
                   <c:v>1212</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2347</c:v>
+                  <c:v>2357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2284,7 +2284,7 @@
                   <c:v>13732</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57049</c:v>
+                  <c:v>63880</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2369,7 +2369,7 @@
                   <c:v>17038</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31114</c:v>
+                  <c:v>33051</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2479,7 +2479,7 @@
                         <c:v>73</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>151</c:v>
+                        <c:v>183</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2584,7 +2584,7 @@
                         <c:v>26</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>251</c:v>
+                        <c:v>271</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2689,7 +2689,7 @@
                         <c:v>1212</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2347</c:v>
+                        <c:v>2357</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3189,7 +3189,7 @@
                   <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>151</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3274,7 +3274,7 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>251</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3384,7 +3384,7 @@
                         <c:v>13732</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>57049</c:v>
+                        <c:v>63880</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3489,7 +3489,7 @@
                         <c:v>17038</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>31114</c:v>
+                        <c:v>33051</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3594,7 +3594,7 @@
                         <c:v>1212</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2347</c:v>
+                        <c:v>2357</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4131,7 +4131,7 @@
                   <c:v>1212</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2347</c:v>
+                  <c:v>2357</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -4243,7 +4243,7 @@
                         <c:v>13732</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>57049</c:v>
+                        <c:v>63880</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4348,7 +4348,7 @@
                         <c:v>73</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>151</c:v>
+                        <c:v>183</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4453,7 +4453,7 @@
                         <c:v>17038</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>31114</c:v>
+                        <c:v>33051</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4558,7 +4558,7 @@
                         <c:v>26</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>251</c:v>
+                        <c:v>271</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -8643,11 +8643,11 @@
   <dimension ref="A1:AF101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-      <selection pane="bottomRight" activeCell="R41" sqref="R41"/>
+      <selection pane="bottomRight" activeCell="L101" sqref="L101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -8819,7 +8819,7 @@
         <v>22081</v>
       </c>
       <c r="L3" s="35">
-        <v>30276</v>
+        <v>32185</v>
       </c>
       <c r="M3" s="87"/>
       <c r="O3" s="35"/>
@@ -8873,7 +8873,7 @@
         <v>71</v>
       </c>
       <c r="L4" s="35">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M4" s="87"/>
       <c r="O4" s="35"/>
@@ -8927,7 +8927,7 @@
         <v>67</v>
       </c>
       <c r="L5" s="35">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M5" s="87"/>
       <c r="O5" s="35"/>
@@ -8981,7 +8981,7 @@
         <v>519</v>
       </c>
       <c r="L6" s="35">
-        <v>637</v>
+        <v>664</v>
       </c>
       <c r="M6" s="87"/>
       <c r="O6" s="35"/>
@@ -9035,7 +9035,7 @@
         <v>108</v>
       </c>
       <c r="L7" s="35">
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="M7" s="87"/>
       <c r="O7" s="35"/>
@@ -9089,7 +9089,7 @@
         <v>1822</v>
       </c>
       <c r="L8" s="35">
-        <v>2347</v>
+        <v>2357</v>
       </c>
       <c r="M8" s="87"/>
       <c r="O8" s="35"/>
@@ -9143,7 +9143,7 @@
         <v>70</v>
       </c>
       <c r="L9" s="35">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="M9" s="87"/>
       <c r="O9" s="35"/>
@@ -9207,7 +9207,7 @@
       </c>
       <c r="L10" s="36">
         <f>L11-SUM(L3:L9)</f>
-        <v>57049</v>
+        <v>63880</v>
       </c>
       <c r="M10" s="88"/>
       <c r="O10" s="36"/>
@@ -9261,7 +9261,7 @@
         <v>53091</v>
       </c>
       <c r="L11" s="38">
-        <v>90912</v>
+        <v>99742</v>
       </c>
       <c r="M11" s="47"/>
       <c r="O11" s="38"/>
@@ -9341,7 +9341,7 @@
       </c>
       <c r="L14" s="55" t="str">
         <f>L2</f>
-        <v>31 สิงหาคม 2566</v>
+        <v>31 กันยายน 2566</v>
       </c>
       <c r="M14" s="89"/>
     </row>
@@ -9377,7 +9377,7 @@
         <v>22282943</v>
       </c>
       <c r="L15" s="35">
-        <v>22464661</v>
+        <v>22490445</v>
       </c>
       <c r="M15" s="87"/>
     </row>
@@ -9413,7 +9413,7 @@
         <v>139682</v>
       </c>
       <c r="L16" s="35">
-        <v>134257</v>
+        <v>133298</v>
       </c>
       <c r="M16" s="87"/>
     </row>
@@ -9449,7 +9449,7 @@
         <v>1358</v>
       </c>
       <c r="L17" s="35">
-        <v>1324</v>
+        <v>1313</v>
       </c>
       <c r="M17" s="87"/>
     </row>
@@ -9485,7 +9485,7 @@
         <v>18443</v>
       </c>
       <c r="L18" s="35">
-        <v>18021</v>
+        <v>17970</v>
       </c>
       <c r="M18" s="87"/>
     </row>
@@ -9521,7 +9521,7 @@
         <v>7098382</v>
       </c>
       <c r="L19" s="35">
-        <v>7108696</v>
+        <v>7109198</v>
       </c>
       <c r="M19" s="87"/>
     </row>
@@ -9557,7 +9557,7 @@
         <v>131155</v>
       </c>
       <c r="L20" s="35">
-        <v>129946</v>
+        <v>129600</v>
       </c>
       <c r="M20" s="87"/>
     </row>
@@ -9593,7 +9593,7 @@
         <v>1227322</v>
       </c>
       <c r="L21" s="35">
-        <v>1238642</v>
+        <v>1241250</v>
       </c>
       <c r="M21" s="87"/>
     </row>
@@ -9639,7 +9639,7 @@
       </c>
       <c r="L22" s="36">
         <f>L23-SUM(L15:L21)</f>
-        <v>13019982</v>
+        <v>13056852</v>
       </c>
       <c r="M22" s="88"/>
     </row>
@@ -9675,7 +9675,7 @@
         <v>43707609</v>
       </c>
       <c r="L23" s="38">
-        <v>44115529</v>
+        <v>44179926</v>
       </c>
       <c r="M23" s="47"/>
     </row>
@@ -9752,7 +9752,7 @@
       </c>
       <c r="L26" s="51" t="str">
         <f>L14</f>
-        <v>31 สิงหาคม 2566</v>
+        <v>31 กันยายน 2566</v>
       </c>
       <c r="M26" s="51" t="s">
         <v>149</v>
@@ -9854,11 +9854,11 @@
       </c>
       <c r="L27" s="40">
         <f>L10</f>
-        <v>57049</v>
+        <v>63880</v>
       </c>
       <c r="M27" s="79">
         <f>L27/L$32</f>
-        <v>0.62751891939457938</v>
+        <v>0.64045236710713638</v>
       </c>
       <c r="O27" s="40">
         <v>1899</v>
@@ -9957,11 +9957,11 @@
       </c>
       <c r="L28" s="40">
         <f t="shared" ref="L28" si="14">L7</f>
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="M28" s="79">
         <f t="shared" ref="M28:M31" si="15">L28/L$32</f>
-        <v>1.6609468497008097E-3</v>
+        <v>1.8347336127208197E-3</v>
       </c>
       <c r="O28" s="40">
         <v>0</v>
@@ -10060,11 +10060,11 @@
       </c>
       <c r="L29" s="40">
         <f t="shared" ref="L29" si="17">SUM(L3:L6)</f>
-        <v>31114</v>
+        <v>33051</v>
       </c>
       <c r="M29" s="79">
         <f t="shared" si="15"/>
-        <v>0.34224304822245688</v>
+        <v>0.33136492149746344</v>
       </c>
       <c r="O29" s="40">
         <v>2593</v>
@@ -10163,11 +10163,11 @@
       </c>
       <c r="L30" s="40">
         <f t="shared" ref="L30" si="19">L9</f>
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="M30" s="79">
         <f t="shared" si="15"/>
-        <v>2.7609116508271734E-3</v>
+        <v>2.7170098855046018E-3</v>
       </c>
       <c r="O30" s="40">
         <v>0</v>
@@ -10266,11 +10266,11 @@
       </c>
       <c r="L31" s="40">
         <f>L8</f>
-        <v>2347</v>
+        <v>2357</v>
       </c>
       <c r="M31" s="79">
         <f t="shared" si="15"/>
-        <v>2.5816173882435761E-2</v>
+        <v>2.3630967897174712E-2</v>
       </c>
       <c r="O31" s="40">
         <v>2</v>
@@ -10369,7 +10369,7 @@
       </c>
       <c r="L32" s="43">
         <f t="shared" ref="L32" si="22">SUM(L27:L31)</f>
-        <v>90912</v>
+        <v>99742</v>
       </c>
       <c r="M32" s="80">
         <f t="shared" ref="M32" si="23">K32/K$32</f>
@@ -10508,7 +10508,7 @@
       </c>
       <c r="L35" s="51" t="str">
         <f t="shared" si="25"/>
-        <v>31 สิงหาคม 2566</v>
+        <v>31 กันยายน 2566</v>
       </c>
       <c r="M35" s="86"/>
       <c r="O35" s="50">
@@ -10605,7 +10605,7 @@
       </c>
       <c r="L36" s="40">
         <f>L27-J27</f>
-        <v>43317</v>
+        <v>50148</v>
       </c>
       <c r="O36" s="79"/>
       <c r="P36" s="40">
@@ -10716,7 +10716,7 @@
       </c>
       <c r="L37" s="40">
         <f t="shared" ref="L37:L41" si="29">L28-J28</f>
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="O37" s="79"/>
       <c r="P37" s="40">
@@ -10827,7 +10827,7 @@
       </c>
       <c r="L38" s="40">
         <f t="shared" si="29"/>
-        <v>14076</v>
+        <v>16013</v>
       </c>
       <c r="O38" s="79"/>
       <c r="P38" s="40">
@@ -10938,7 +10938,7 @@
       </c>
       <c r="L39" s="40">
         <f t="shared" si="29"/>
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="O39" s="79"/>
       <c r="P39" s="40">
@@ -11049,7 +11049,7 @@
       </c>
       <c r="L40" s="40">
         <f t="shared" si="29"/>
-        <v>1135</v>
+        <v>1145</v>
       </c>
       <c r="O40" s="79"/>
       <c r="P40" s="40">
@@ -11160,7 +11160,7 @@
       </c>
       <c r="L41" s="43">
         <f t="shared" si="29"/>
-        <v>58831</v>
+        <v>67661</v>
       </c>
       <c r="O41" s="80"/>
       <c r="P41" s="43">
@@ -11293,7 +11293,7 @@
       </c>
       <c r="L44" s="51" t="str">
         <f t="shared" si="39"/>
-        <v>31 สิงหาคม 2566</v>
+        <v>31 กันยายน 2566</v>
       </c>
       <c r="M44" s="86"/>
       <c r="O44" s="50">
@@ -11390,7 +11390,7 @@
       </c>
       <c r="L45" s="79">
         <f>IF(L27*J27=0,"",L27/J27-1)</f>
-        <v>3.1544567433731432</v>
+        <v>3.6519079522283713</v>
       </c>
       <c r="M45" s="90"/>
       <c r="O45" s="79"/>
@@ -11502,7 +11502,7 @@
       </c>
       <c r="L46" s="79">
         <f t="shared" ref="L46:L50" si="43">IF(L28*J28=0,"",L28/J28-1)</f>
-        <v>1.0684931506849313</v>
+        <v>1.506849315068493</v>
       </c>
       <c r="M46" s="90"/>
       <c r="O46" s="79"/>
@@ -11614,7 +11614,7 @@
       </c>
       <c r="L47" s="79">
         <f t="shared" si="43"/>
-        <v>0.82615330437844814</v>
+        <v>0.93984035684939538</v>
       </c>
       <c r="M47" s="90"/>
       <c r="O47" s="79"/>
@@ -11726,7 +11726,7 @@
       </c>
       <c r="L48" s="79">
         <f t="shared" si="43"/>
-        <v>8.6538461538461533</v>
+        <v>9.4230769230769234</v>
       </c>
       <c r="M48" s="90"/>
       <c r="O48" s="79"/>
@@ -11838,7 +11838,7 @@
       </c>
       <c r="L49" s="79">
         <f t="shared" si="43"/>
-        <v>0.93646864686468656</v>
+        <v>0.94471947194719474</v>
       </c>
       <c r="M49" s="90"/>
       <c r="O49" s="79"/>
@@ -11950,7 +11950,7 @@
       </c>
       <c r="L50" s="80">
         <f t="shared" si="43"/>
-        <v>1.8338268757208316</v>
+        <v>2.1090676724541004</v>
       </c>
       <c r="M50" s="90"/>
       <c r="O50" s="80"/>
@@ -12085,7 +12085,7 @@
       </c>
       <c r="L52" s="55" t="str">
         <f t="shared" si="53"/>
-        <v>31 สิงหาคม 2566</v>
+        <v>31 กันยายน 2566</v>
       </c>
       <c r="M52" s="55" t="s">
         <v>149</v>
@@ -12134,11 +12134,11 @@
       </c>
       <c r="L53" s="40">
         <f t="shared" ref="L53" si="55">L22</f>
-        <v>13019982</v>
+        <v>13056852</v>
       </c>
       <c r="M53" s="79">
         <f>L53/L$58</f>
-        <v>0.29513376117511819</v>
+        <v>0.29553811384835726</v>
       </c>
     </row>
     <row r="54" spans="2:32" x14ac:dyDescent="0.35">
@@ -12183,11 +12183,11 @@
       </c>
       <c r="L54" s="40">
         <f t="shared" ref="L54" si="57">L19</f>
-        <v>7108696</v>
+        <v>7109198</v>
       </c>
       <c r="M54" s="79">
         <f t="shared" ref="M54:M57" si="58">L54/L$58</f>
-        <v>0.16113817880320555</v>
+        <v>0.16091466518074293</v>
       </c>
     </row>
     <row r="55" spans="2:32" x14ac:dyDescent="0.35">
@@ -12232,11 +12232,11 @@
       </c>
       <c r="L55" s="40">
         <f t="shared" ref="L55" si="60">SUM(L15:L18)</f>
-        <v>22618263</v>
+        <v>22643026</v>
       </c>
       <c r="M55" s="79">
         <f t="shared" si="58"/>
-        <v>0.51270524263689554</v>
+        <v>0.512518422959785</v>
       </c>
     </row>
     <row r="56" spans="2:32" x14ac:dyDescent="0.35">
@@ -12281,11 +12281,11 @@
       </c>
       <c r="L56" s="40">
         <f t="shared" ref="L56" si="62">L21</f>
-        <v>1238642</v>
+        <v>1241250</v>
       </c>
       <c r="M56" s="79">
         <f t="shared" si="58"/>
-        <v>2.8077233302586036E-2</v>
+        <v>2.8095339046063591E-2</v>
       </c>
     </row>
     <row r="57" spans="2:32" x14ac:dyDescent="0.35">
@@ -12330,11 +12330,11 @@
       </c>
       <c r="L57" s="40">
         <f t="shared" ref="L57" si="64">L20</f>
-        <v>129946</v>
+        <v>129600</v>
       </c>
       <c r="M57" s="79">
         <f t="shared" si="58"/>
-        <v>2.94558408219473E-3</v>
+        <v>2.9334589650512315E-3</v>
       </c>
     </row>
     <row r="58" spans="2:32" x14ac:dyDescent="0.35">
@@ -12379,7 +12379,7 @@
       </c>
       <c r="L58" s="43">
         <f t="shared" ref="L58" si="66">SUM(L53:L57)</f>
-        <v>44115529</v>
+        <v>44179926</v>
       </c>
       <c r="M58" s="80">
         <f t="shared" ref="M58" si="67">K58/K$58</f>
@@ -12428,7 +12428,7 @@
       </c>
       <c r="L60" s="66" t="str">
         <f t="shared" si="68"/>
-        <v>31 สิงหาคม 2566</v>
+        <v>31 กันยายน 2566</v>
       </c>
       <c r="M60" s="91"/>
     </row>
@@ -12474,7 +12474,7 @@
       </c>
       <c r="L61" s="44">
         <f t="shared" ref="L61" si="70">L27/L53</f>
-        <v>4.3816496827722186E-3</v>
+        <v>4.8924503394845867E-3</v>
       </c>
       <c r="M61" s="92"/>
     </row>
@@ -12520,7 +12520,7 @@
       </c>
       <c r="L62" s="44">
         <f t="shared" ref="L62" si="72">L28/L54</f>
-        <v>2.1241589174723466E-5</v>
+        <v>2.5741300214173243E-5</v>
       </c>
       <c r="M62" s="92"/>
     </row>
@@ -12566,7 +12566,7 @@
       </c>
       <c r="L63" s="44">
         <f t="shared" ref="L63" si="74">L29/L55</f>
-        <v>1.3756140336682796E-3</v>
+        <v>1.4596547298934338E-3</v>
       </c>
       <c r="M63" s="92"/>
     </row>
@@ -12612,7 +12612,7 @@
       </c>
       <c r="L64" s="44">
         <f t="shared" ref="L64" si="76">L30/L56</f>
-        <v>2.0264127972408492E-4</v>
+        <v>2.1832829808660623E-4</v>
       </c>
       <c r="M64" s="92"/>
     </row>
@@ -12658,7 +12658,7 @@
       </c>
       <c r="L65" s="44">
         <f t="shared" ref="L65" si="78">L31/L57</f>
-        <v>1.8061348560171147E-2</v>
+        <v>1.8186728395061729E-2</v>
       </c>
       <c r="M65" s="92"/>
     </row>
@@ -12704,7 +12704,7 @@
       </c>
       <c r="L66" s="45">
         <f t="shared" ref="L66" si="80">L32/L58</f>
-        <v>2.0607709362388017E-3</v>
+        <v>2.2576316673776232E-3</v>
       </c>
       <c r="M66" s="92"/>
     </row>
@@ -12755,7 +12755,7 @@
       </c>
       <c r="L69" s="55" t="str">
         <f t="shared" si="81"/>
-        <v>31 สิงหาคม 2566</v>
+        <v>31 กันยายน 2566</v>
       </c>
       <c r="M69" s="55" t="s">
         <v>149</v>
@@ -12803,7 +12803,7 @@
       </c>
       <c r="L70" s="40">
         <f t="shared" si="83"/>
-        <v>13019982</v>
+        <v>13056852</v>
       </c>
       <c r="M70" s="79"/>
     </row>
@@ -12849,7 +12849,7 @@
       </c>
       <c r="L71" s="40">
         <f t="shared" si="85"/>
-        <v>7108696</v>
+        <v>7109198</v>
       </c>
       <c r="M71" s="79"/>
     </row>
@@ -12895,7 +12895,7 @@
       </c>
       <c r="L72" s="40">
         <f t="shared" si="87"/>
-        <v>22618263</v>
+        <v>22643026</v>
       </c>
       <c r="M72" s="79"/>
     </row>
@@ -12941,7 +12941,7 @@
       </c>
       <c r="L73" s="40">
         <f t="shared" si="89"/>
-        <v>1238642</v>
+        <v>1241250</v>
       </c>
       <c r="M73" s="79"/>
     </row>
@@ -12987,7 +12987,7 @@
       </c>
       <c r="L74" s="40">
         <f t="shared" si="91"/>
-        <v>129946</v>
+        <v>129600</v>
       </c>
       <c r="M74" s="79"/>
     </row>
@@ -13033,7 +13033,7 @@
       </c>
       <c r="L75" s="43">
         <f t="shared" si="93"/>
-        <v>44115529</v>
+        <v>44179926</v>
       </c>
       <c r="M75" s="80"/>
     </row>
@@ -13088,7 +13088,7 @@
       </c>
       <c r="L78" s="54" t="str">
         <f t="shared" si="94"/>
-        <v>31 สิงหาคม 2566</v>
+        <v>31 กันยายน 2566</v>
       </c>
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.35">
@@ -13130,7 +13130,7 @@
       </c>
       <c r="L79" s="40">
         <f>L70-J70</f>
-        <v>370862</v>
+        <v>407732</v>
       </c>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.35">
@@ -13172,7 +13172,7 @@
       </c>
       <c r="L80" s="40">
         <f t="shared" ref="L80:L84" si="103">L71-J71</f>
-        <v>22786</v>
+        <v>23288</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.35">
@@ -13214,7 +13214,7 @@
       </c>
       <c r="L81" s="40">
         <f t="shared" si="103"/>
-        <v>317544</v>
+        <v>342307</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.35">
@@ -13256,7 +13256,7 @@
       </c>
       <c r="L82" s="40">
         <f t="shared" si="103"/>
-        <v>13093</v>
+        <v>15701</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.35">
@@ -13298,7 +13298,7 @@
       </c>
       <c r="L83" s="40">
         <f t="shared" si="103"/>
-        <v>-2860</v>
+        <v>-3206</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.35">
@@ -13340,7 +13340,7 @@
       </c>
       <c r="L84" s="43">
         <f t="shared" si="103"/>
-        <v>721425</v>
+        <v>785822</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.35">
@@ -13394,7 +13394,7 @@
       </c>
       <c r="L87" s="54" t="str">
         <f t="shared" si="104"/>
-        <v>31 สิงหาคม 2566</v>
+        <v>31 กันยายน 2566</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.35">
@@ -13436,7 +13436,7 @@
       </c>
       <c r="L88" s="79">
         <f>IF(L70*J70=0,"",L70/J70-1)</f>
-        <v>2.9319193746284222E-2</v>
+        <v>3.2234021022806258E-2</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.35">
@@ -13478,7 +13478,7 @@
       </c>
       <c r="L89" s="79">
         <f t="shared" ref="L89:L93" si="113">IF(L71*J71=0,"",L71/J71-1)</f>
-        <v>3.2156773089131452E-3</v>
+        <v>3.2865221263040922E-3</v>
       </c>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.35">
@@ -13520,7 +13520,7 @@
       </c>
       <c r="L90" s="79">
         <f t="shared" si="113"/>
-        <v>1.4239182153723329E-2</v>
+        <v>1.5349594782123388E-2</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.35">
@@ -13562,7 +13562,7 @@
       </c>
       <c r="L91" s="79">
         <f t="shared" si="113"/>
-        <v>1.0683375368916392E-2</v>
+        <v>1.2811401257722066E-2</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.35">
@@ -13604,7 +13604,7 @@
       </c>
       <c r="L92" s="79">
         <f t="shared" si="113"/>
-        <v>-2.153517160369256E-2</v>
+        <v>-2.4140475580922582E-2</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.35">
@@ -13646,7 +13646,7 @@
       </c>
       <c r="L93" s="80">
         <f t="shared" si="113"/>
-        <v>1.662495439472611E-2</v>
+        <v>1.8108957843673945E-2</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.35">
@@ -13691,7 +13691,7 @@
       </c>
       <c r="L95" s="66" t="str">
         <f t="shared" ref="L95" si="115">L44</f>
-        <v>31 สิงหาคม 2566</v>
+        <v>31 กันยายน 2566</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.35">
@@ -13733,7 +13733,7 @@
       </c>
       <c r="L96" s="44">
         <f>L36/L79</f>
-        <v>0.1168008585403735</v>
+        <v>0.12299255393248507</v>
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.35">
@@ -13775,7 +13775,7 @@
       </c>
       <c r="L97" s="44">
         <f t="shared" ref="L97:L101" si="117">L37/L80</f>
-        <v>3.423154568594751E-3</v>
+        <v>4.7234627275850221E-3</v>
       </c>
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.35">
@@ -13817,7 +13817,7 @@
       </c>
       <c r="L98" s="44">
         <f t="shared" si="117"/>
-        <v>4.4327715214269515E-2</v>
+        <v>4.677964517231608E-2</v>
       </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.35">
@@ -13859,7 +13859,7 @@
       </c>
       <c r="L99" s="44">
         <f t="shared" si="117"/>
-        <v>1.7184755212709082E-2</v>
+        <v>1.5604101649576461E-2</v>
       </c>
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.35">
@@ -13901,7 +13901,7 @@
       </c>
       <c r="L100" s="44">
         <f t="shared" si="117"/>
-        <v>-0.39685314685314688</v>
+        <v>-0.35714285714285715</v>
       </c>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.35">
@@ -13943,7 +13943,7 @@
       </c>
       <c r="L101" s="45">
         <f t="shared" si="117"/>
-        <v>8.154832449665593E-2</v>
+        <v>8.6102196171652101E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update EV vehicle to december 2023
</commit_message>
<xml_diff>
--- a/rawdata/01 EGAT_EV_เตรียมข้อมูลประชุม_Sep2023.xlsx
+++ b/rawdata/01 EGAT_EV_เตรียมข้อมูลประชุม_Sep2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rstudio\thailandVehicleAnalysis\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F617BE2B-BA3A-418E-A4F7-7E0C782EE485}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015E09AC-0DC6-4FEC-9BD1-3E17F08B92AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="2" activeTab="2" xr2:uid="{EDD8F08D-6CA6-4516-B97F-8A475C3F3159}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="M3_Timeline" sheetId="4" r:id="rId4"/>
     <sheet name="M3_สรุปโครงการ" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="151">
   <si>
     <t>ELEX</t>
   </si>
@@ -1002,20 +1002,17 @@
   <si>
     <t>ส่วนเพิ่ม BEV/รถทุกเชื้อเพลิง</t>
   </si>
-  <si>
-    <t>31 กันยายน 2566</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="187" formatCode="B1mmm\-yy"/>
-    <numFmt numFmtId="188" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="189" formatCode="[$-107041E]d\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="190" formatCode="0.0%"/>
+    <numFmt numFmtId="187" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="188" formatCode="B1mmm\-yy"/>
+    <numFmt numFmtId="189" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="190" formatCode="[$-107041E]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="191" formatCode="0.0%"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -1308,11 +1305,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1331,7 +1328,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="187" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1343,36 +1340,36 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="4" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="4" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="190" fontId="5" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="190" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="191" fontId="5" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="191" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1382,7 +1379,7 @@
     <xf numFmtId="1" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1394,12 +1391,12 @@
     <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="7" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="7" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1417,7 +1414,7 @@
     <xf numFmtId="1" fontId="7" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="7" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="7" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1448,10 +1445,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="188" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="188" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1460,27 +1457,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="188" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="188" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="189" fontId="7" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="7" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="188" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="189" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="190" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="7" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="7" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="190" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="7" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="191" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1548,9 +1542,10 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>M3_BEV!$C$26:$L$26</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2558</c:v>
@@ -1577,10 +1572,10 @@
                   <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31 กันยายน 2566</c:v>
+                  <c:v>2566</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1613,7 +1608,7 @@
                   <c:v>13732</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>63880</c:v>
+                  <c:v>89743</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1652,9 +1647,10 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>M3_BEV!$C$26:$L$26</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2558</c:v>
@@ -1681,10 +1677,10 @@
                   <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31 กันยายน 2566</c:v>
+                  <c:v>2566</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1717,7 +1713,7 @@
                   <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>183</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1756,9 +1752,10 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>M3_BEV!$C$26:$L$26</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2558</c:v>
@@ -1785,10 +1782,10 @@
                   <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31 กันยายน 2566</c:v>
+                  <c:v>2566</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1821,7 +1818,7 @@
                   <c:v>17038</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33051</c:v>
+                  <c:v>39112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1860,9 +1857,10 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>M3_BEV!$C$26:$L$26</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2558</c:v>
@@ -1889,10 +1887,10 @@
                   <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31 กันยายน 2566</c:v>
+                  <c:v>2566</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1925,7 +1923,7 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>271</c:v>
+                  <c:v>303</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1964,9 +1962,10 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>M3_BEV!$C$26:$L$26</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2558</c:v>
@@ -1993,10 +1992,10 @@
                   <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31 กันยายน 2566</c:v>
+                  <c:v>2566</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2029,7 +2028,7 @@
                   <c:v>1212</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2357</c:v>
+                  <c:v>2419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2060,7 +2059,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2284,7 +2283,7 @@
                   <c:v>13732</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63880</c:v>
+                  <c:v>89743</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2369,7 +2368,7 @@
                   <c:v>17038</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33051</c:v>
+                  <c:v>39112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2479,7 +2478,7 @@
                         <c:v>73</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>183</c:v>
+                        <c:v>279</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2584,7 +2583,7 @@
                         <c:v>26</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>271</c:v>
+                        <c:v>303</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2689,7 +2688,7 @@
                         <c:v>1212</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2357</c:v>
+                        <c:v>2419</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3189,7 +3188,7 @@
                   <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>183</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3274,7 +3273,7 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>271</c:v>
+                  <c:v>303</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3384,7 +3383,7 @@
                         <c:v>13732</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>63880</c:v>
+                        <c:v>89743</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3489,7 +3488,7 @@
                         <c:v>17038</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>33051</c:v>
+                        <c:v>39112</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3594,7 +3593,7 @@
                         <c:v>1212</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2357</c:v>
+                        <c:v>2419</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4131,7 +4130,7 @@
                   <c:v>1212</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2357</c:v>
+                  <c:v>2419</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -4243,7 +4242,7 @@
                         <c:v>13732</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>63880</c:v>
+                        <c:v>89743</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4348,7 +4347,7 @@
                         <c:v>73</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>183</c:v>
+                        <c:v>279</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4453,7 +4452,7 @@
                         <c:v>17038</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>33051</c:v>
+                        <c:v>39112</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4558,7 +4557,7 @@
                         <c:v>26</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>271</c:v>
+                        <c:v>303</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -7335,16 +7334,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>143436</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257734</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>121025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>434788</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>89648</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>468405</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7833,164 +7832,164 @@
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="61" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" s="62" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B12" s="63" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B14" s="62" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="63" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="63" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" s="63" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="63" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>84</v>
       </c>
@@ -8009,20 +8008,20 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.69921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
@@ -8063,7 +8062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
@@ -8105,7 +8104,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
@@ -8151,7 +8150,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
@@ -8197,7 +8196,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
@@ -8243,7 +8242,7 @@
         <v>0.20340501792114685</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
@@ -8251,7 +8250,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -8260,7 +8259,7 @@
         <v>1.2034050179211468</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
         <v>24</v>
       </c>
@@ -8280,7 +8279,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="16" t="s">
         <v>19</v>
       </c>
@@ -8300,7 +8299,7 @@
         <v>7325</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="17" t="s">
         <v>20</v>
       </c>
@@ -8320,7 +8319,7 @@
         <v>5947</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
         <v>21</v>
       </c>
@@ -8340,7 +8339,7 @@
         <v>32718</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>22</v>
       </c>
@@ -8360,7 +8359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>23</v>
       </c>
@@ -8385,7 +8384,7 @@
         <v>45990</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="15" t="s">
         <v>25</v>
       </c>
@@ -8405,7 +8404,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="16" t="s">
         <v>19</v>
       </c>
@@ -8432,7 +8431,7 @@
         <v>21.805847953216375</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="17" t="s">
         <v>20</v>
       </c>
@@ -8448,7 +8447,7 @@
         <v>37075</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
         <v>21</v>
       </c>
@@ -8464,7 +8463,7 @@
         <v>228894</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="11" t="s">
         <v>22</v>
       </c>
@@ -8478,7 +8477,7 @@
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
         <v>23</v>
       </c>
@@ -8503,7 +8502,7 @@
         <v>284613</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="13" t="s">
         <v>31</v>
       </c>
@@ -8520,7 +8519,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
@@ -8538,7 +8537,7 @@
         <v>264361</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
@@ -8556,7 +8555,7 @@
         <v>19570</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
@@ -8574,7 +8573,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
@@ -8592,7 +8591,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
@@ -8610,7 +8609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>32</v>
       </c>
@@ -8643,41 +8642,41 @@
   <dimension ref="A1:AF101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-      <selection pane="bottomRight" activeCell="L101" sqref="L101"/>
+      <selection pane="bottomRight" activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.69921875" style="32"/>
-    <col min="2" max="2" width="22.8984375" style="30" customWidth="1"/>
-    <col min="3" max="3" width="12.69921875" style="31" customWidth="1"/>
-    <col min="4" max="10" width="12.59765625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="8.75" style="32"/>
+    <col min="2" max="2" width="22.875" style="30" customWidth="1"/>
+    <col min="3" max="3" width="12.75" style="31" customWidth="1"/>
+    <col min="4" max="10" width="12.625" style="31" customWidth="1"/>
     <col min="11" max="11" width="13.5" style="31" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.19921875" style="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.25" style="31" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" style="31" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="8.69921875" style="32"/>
+    <col min="14" max="15" width="8.75" style="32"/>
     <col min="16" max="16" width="8" style="32" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.8984375" style="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.875" style="32" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="32" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.8984375" style="32" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.875" style="32" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" style="32" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.8984375" style="32" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="8.69921875" style="32" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="8.75" style="32" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="9" style="32" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.8984375" style="32" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.09765625" style="32" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.8984375" style="32" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="9.69921875" style="32" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.8984375" style="32" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.19921875" style="32" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.69921875" style="32"/>
+    <col min="26" max="26" width="8.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.125" style="32" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="9.75" style="32" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.25" style="32" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="8.75" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B1" s="59" t="s">
         <v>49</v>
       </c>
@@ -8690,7 +8689,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="2:32" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:32" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="49" t="s">
         <v>51</v>
       </c>
@@ -8702,7 +8701,7 @@
         <v>2559</v>
       </c>
       <c r="E2" s="50">
-        <f t="shared" ref="E2:J2" si="0">D2+1</f>
+        <f t="shared" ref="E2:L2" si="0">D2+1</f>
         <v>2560</v>
       </c>
       <c r="F2" s="50">
@@ -8728,8 +8727,8 @@
       <c r="K2" s="51">
         <v>45016</v>
       </c>
-      <c r="L2" s="93" t="s">
-        <v>151</v>
+      <c r="L2" s="50">
+        <v>2566</v>
       </c>
       <c r="M2" s="86"/>
       <c r="O2" s="50">
@@ -8787,7 +8786,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="3" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B3" s="34" t="s">
         <v>38</v>
       </c>
@@ -8819,7 +8818,7 @@
         <v>22081</v>
       </c>
       <c r="L3" s="35">
-        <v>32185</v>
+        <v>38076</v>
       </c>
       <c r="M3" s="87"/>
       <c r="O3" s="35"/>
@@ -8841,7 +8840,7 @@
       <c r="AE3" s="35"/>
       <c r="AF3" s="35"/>
     </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B4" s="34" t="s">
         <v>39</v>
       </c>
@@ -8873,7 +8872,7 @@
         <v>71</v>
       </c>
       <c r="L4" s="35">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="M4" s="87"/>
       <c r="O4" s="35"/>
@@ -8895,7 +8894,7 @@
       <c r="AE4" s="35"/>
       <c r="AF4" s="35"/>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B5" s="34" t="s">
         <v>36</v>
       </c>
@@ -8927,7 +8926,7 @@
         <v>67</v>
       </c>
       <c r="L5" s="35">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M5" s="87"/>
       <c r="O5" s="35"/>
@@ -8949,7 +8948,7 @@
       <c r="AE5" s="35"/>
       <c r="AF5" s="35"/>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B6" s="34" t="s">
         <v>37</v>
       </c>
@@ -8981,7 +8980,7 @@
         <v>519</v>
       </c>
       <c r="L6" s="35">
-        <v>664</v>
+        <v>821</v>
       </c>
       <c r="M6" s="87"/>
       <c r="O6" s="35"/>
@@ -9003,7 +9002,7 @@
       <c r="AE6" s="35"/>
       <c r="AF6" s="35"/>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B7" s="76" t="s">
         <v>136</v>
       </c>
@@ -9035,7 +9034,7 @@
         <v>108</v>
       </c>
       <c r="L7" s="35">
-        <v>183</v>
+        <v>279</v>
       </c>
       <c r="M7" s="87"/>
       <c r="O7" s="35"/>
@@ -9057,7 +9056,7 @@
       <c r="AE7" s="35"/>
       <c r="AF7" s="35"/>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B8" s="76" t="s">
         <v>135</v>
       </c>
@@ -9089,7 +9088,7 @@
         <v>1822</v>
       </c>
       <c r="L8" s="35">
-        <v>2357</v>
+        <v>2419</v>
       </c>
       <c r="M8" s="87"/>
       <c r="O8" s="35"/>
@@ -9111,7 +9110,7 @@
       <c r="AE8" s="35"/>
       <c r="AF8" s="35"/>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B9" s="76" t="s">
         <v>134</v>
       </c>
@@ -9143,7 +9142,7 @@
         <v>70</v>
       </c>
       <c r="L9" s="35">
-        <v>271</v>
+        <v>303</v>
       </c>
       <c r="M9" s="87"/>
       <c r="O9" s="35"/>
@@ -9165,7 +9164,7 @@
       <c r="AE9" s="35"/>
       <c r="AF9" s="35"/>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B10" s="75" t="s">
         <v>42</v>
       </c>
@@ -9207,7 +9206,7 @@
       </c>
       <c r="L10" s="36">
         <f>L11-SUM(L3:L9)</f>
-        <v>63880</v>
+        <v>89743</v>
       </c>
       <c r="M10" s="88"/>
       <c r="O10" s="36"/>
@@ -9229,7 +9228,7 @@
       <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
     </row>
-    <row r="11" spans="2:32" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:32" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="37" t="s">
         <v>35</v>
       </c>
@@ -9261,7 +9260,7 @@
         <v>53091</v>
       </c>
       <c r="L11" s="38">
-        <v>99742</v>
+        <v>131856</v>
       </c>
       <c r="M11" s="47"/>
       <c r="O11" s="38"/>
@@ -9283,7 +9282,7 @@
       <c r="AE11" s="38"/>
       <c r="AF11" s="38"/>
     </row>
-    <row r="12" spans="2:32" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:32" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="46" t="s">
         <v>48</v>
       </c>
@@ -9299,7 +9298,7 @@
       <c r="L12" s="47"/>
       <c r="M12" s="47"/>
     </row>
-    <row r="14" spans="2:32" s="52" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:32" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="53" t="s">
         <v>52</v>
       </c>
@@ -9339,13 +9338,13 @@
         <f>K2</f>
         <v>45016</v>
       </c>
-      <c r="L14" s="55" t="str">
+      <c r="L14" s="54">
         <f>L2</f>
-        <v>31 กันยายน 2566</v>
+        <v>2566</v>
       </c>
       <c r="M14" s="89"/>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B15" s="34" t="s">
         <v>38</v>
       </c>
@@ -9377,11 +9376,11 @@
         <v>22282943</v>
       </c>
       <c r="L15" s="35">
-        <v>22490445</v>
+        <v>22569593</v>
       </c>
       <c r="M15" s="87"/>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B16" s="34" t="s">
         <v>39</v>
       </c>
@@ -9413,11 +9412,11 @@
         <v>139682</v>
       </c>
       <c r="L16" s="35">
-        <v>133298</v>
+        <v>130930</v>
       </c>
       <c r="M16" s="87"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B17" s="34" t="s">
         <v>36</v>
       </c>
@@ -9449,11 +9448,11 @@
         <v>1358</v>
       </c>
       <c r="L17" s="35">
-        <v>1313</v>
+        <v>1323</v>
       </c>
       <c r="M17" s="87"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B18" s="34" t="s">
         <v>37</v>
       </c>
@@ -9485,11 +9484,11 @@
         <v>18443</v>
       </c>
       <c r="L18" s="35">
-        <v>17970</v>
+        <v>17847</v>
       </c>
       <c r="M18" s="87"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B19" s="76" t="s">
         <v>136</v>
       </c>
@@ -9521,11 +9520,11 @@
         <v>7098382</v>
       </c>
       <c r="L19" s="35">
-        <v>7109198</v>
+        <v>7106524</v>
       </c>
       <c r="M19" s="87"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B20" s="34" t="s">
         <v>40</v>
       </c>
@@ -9557,11 +9556,11 @@
         <v>131155</v>
       </c>
       <c r="L20" s="35">
-        <v>129600</v>
+        <v>129235</v>
       </c>
       <c r="M20" s="87"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B21" s="34" t="s">
         <v>41</v>
       </c>
@@ -9593,11 +9592,11 @@
         <v>1227322</v>
       </c>
       <c r="L21" s="35">
-        <v>1241250</v>
+        <v>1247128</v>
       </c>
       <c r="M21" s="87"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B22" s="75" t="s">
         <v>42</v>
       </c>
@@ -9639,11 +9638,11 @@
       </c>
       <c r="L22" s="36">
         <f>L23-SUM(L15:L21)</f>
-        <v>13056852</v>
+        <v>13161395</v>
       </c>
       <c r="M22" s="88"/>
     </row>
-    <row r="23" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="37" t="s">
         <v>43</v>
       </c>
@@ -9675,11 +9674,11 @@
         <v>43707609</v>
       </c>
       <c r="L23" s="38">
-        <v>44179926</v>
+        <v>44363975</v>
       </c>
       <c r="M23" s="47"/>
     </row>
-    <row r="24" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="56"/>
       <c r="B24" s="57"/>
       <c r="C24" s="58"/>
@@ -9697,7 +9696,7 @@
       <c r="O24" s="56"/>
       <c r="P24" s="56"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B25" s="60" t="s">
         <v>50</v>
       </c>
@@ -9710,7 +9709,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B26" s="49" t="s">
         <v>51</v>
       </c>
@@ -9750,9 +9749,9 @@
         <f t="shared" si="11"/>
         <v>45016</v>
       </c>
-      <c r="L26" s="51" t="str">
+      <c r="L26" s="50">
         <f>L14</f>
-        <v>31 กันยายน 2566</v>
+        <v>2566</v>
       </c>
       <c r="M26" s="51" t="s">
         <v>149</v>
@@ -9812,7 +9811,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B27" s="39" t="s">
         <v>42</v>
       </c>
@@ -9854,11 +9853,11 @@
       </c>
       <c r="L27" s="40">
         <f>L10</f>
-        <v>63880</v>
+        <v>89743</v>
       </c>
       <c r="M27" s="79">
         <f>L27/L$32</f>
-        <v>0.64045236710713638</v>
+        <v>0.68061369979371433</v>
       </c>
       <c r="O27" s="40">
         <v>1899</v>
@@ -9915,7 +9914,7 @@
         <v>7216379</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B28" s="41" t="s">
         <v>137</v>
       </c>
@@ -9957,11 +9956,11 @@
       </c>
       <c r="L28" s="40">
         <f t="shared" ref="L28" si="14">L7</f>
-        <v>183</v>
+        <v>279</v>
       </c>
       <c r="M28" s="79">
         <f t="shared" ref="M28:M31" si="15">L28/L$32</f>
-        <v>1.8347336127208197E-3</v>
+        <v>2.1159446669093557E-3</v>
       </c>
       <c r="O28" s="40">
         <v>0</v>
@@ -10018,7 +10017,7 @@
         <v>2232662</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B29" s="41" t="s">
         <v>138</v>
       </c>
@@ -10060,11 +10059,11 @@
       </c>
       <c r="L29" s="40">
         <f t="shared" ref="L29" si="17">SUM(L3:L6)</f>
-        <v>33051</v>
+        <v>39112</v>
       </c>
       <c r="M29" s="79">
         <f t="shared" si="15"/>
-        <v>0.33136492149746344</v>
+        <v>0.29662662298264775</v>
       </c>
       <c r="O29" s="40">
         <v>2593</v>
@@ -10121,7 +10120,7 @@
         <v>14603170</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B30" s="39" t="s">
         <v>45</v>
       </c>
@@ -10163,11 +10162,11 @@
       </c>
       <c r="L30" s="40">
         <f t="shared" ref="L30" si="19">L9</f>
-        <v>271</v>
+        <v>303</v>
       </c>
       <c r="M30" s="79">
         <f t="shared" si="15"/>
-        <v>2.7170098855046018E-3</v>
+        <v>2.2979614124499456E-3</v>
       </c>
       <c r="O30" s="40">
         <v>0</v>
@@ -10224,7 +10223,7 @@
         <v>604087</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B31" s="39" t="s">
         <v>46</v>
       </c>
@@ -10266,11 +10265,11 @@
       </c>
       <c r="L31" s="40">
         <f>L8</f>
-        <v>2357</v>
+        <v>2419</v>
       </c>
       <c r="M31" s="79">
         <f t="shared" si="15"/>
-        <v>2.3630967897174712E-2</v>
+        <v>1.8345771144278607E-2</v>
       </c>
       <c r="O31" s="40">
         <v>2</v>
@@ -10327,7 +10326,7 @@
         <v>88736</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B32" s="42" t="s">
         <v>47</v>
       </c>
@@ -10369,7 +10368,7 @@
       </c>
       <c r="L32" s="43">
         <f t="shared" ref="L32" si="22">SUM(L27:L31)</f>
-        <v>99742</v>
+        <v>131856</v>
       </c>
       <c r="M32" s="80">
         <f t="shared" ref="M32" si="23">K32/K$32</f>
@@ -10448,12 +10447,12 @@
         <v>24745034</v>
       </c>
     </row>
-    <row r="33" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:32" x14ac:dyDescent="0.3">
       <c r="O33" s="78" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B34" s="59" t="s">
         <v>144</v>
       </c>
@@ -10466,7 +10465,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B35" s="49" t="s">
         <v>51</v>
       </c>
@@ -10506,9 +10505,9 @@
         <f t="shared" si="25"/>
         <v>45016</v>
       </c>
-      <c r="L35" s="51" t="str">
+      <c r="L35" s="50">
         <f t="shared" si="25"/>
-        <v>31 กันยายน 2566</v>
+        <v>2566</v>
       </c>
       <c r="M35" s="86"/>
       <c r="O35" s="50">
@@ -10566,7 +10565,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="36" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B36" s="39" t="s">
         <v>42</v>
       </c>
@@ -10605,7 +10604,7 @@
       </c>
       <c r="L36" s="40">
         <f>L27-J27</f>
-        <v>50148</v>
+        <v>76011</v>
       </c>
       <c r="O36" s="79"/>
       <c r="P36" s="40">
@@ -10677,7 +10676,7 @@
         <v>1137838</v>
       </c>
     </row>
-    <row r="37" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B37" s="41" t="s">
         <v>137</v>
       </c>
@@ -10716,7 +10715,7 @@
       </c>
       <c r="L37" s="40">
         <f t="shared" ref="L37:L41" si="29">L28-J28</f>
-        <v>110</v>
+        <v>206</v>
       </c>
       <c r="O37" s="79"/>
       <c r="P37" s="40">
@@ -10788,7 +10787,7 @@
         <v>339272</v>
       </c>
     </row>
-    <row r="38" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B38" s="41" t="s">
         <v>138</v>
       </c>
@@ -10827,7 +10826,7 @@
       </c>
       <c r="L38" s="40">
         <f t="shared" si="29"/>
-        <v>16013</v>
+        <v>22074</v>
       </c>
       <c r="O38" s="79"/>
       <c r="P38" s="40">
@@ -10899,7 +10898,7 @@
         <v>2293595</v>
       </c>
     </row>
-    <row r="39" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B39" s="39" t="s">
         <v>45</v>
       </c>
@@ -10938,7 +10937,7 @@
       </c>
       <c r="L39" s="40">
         <f t="shared" si="29"/>
-        <v>245</v>
+        <v>277</v>
       </c>
       <c r="O39" s="79"/>
       <c r="P39" s="40">
@@ -11010,7 +11009,7 @@
         <v>91351</v>
       </c>
     </row>
-    <row r="40" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B40" s="39" t="s">
         <v>46</v>
       </c>
@@ -11049,7 +11048,7 @@
       </c>
       <c r="L40" s="40">
         <f t="shared" si="29"/>
-        <v>1145</v>
+        <v>1207</v>
       </c>
       <c r="O40" s="79"/>
       <c r="P40" s="40">
@@ -11121,7 +11120,7 @@
         <v>13134</v>
       </c>
     </row>
-    <row r="41" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B41" s="42" t="s">
         <v>47</v>
       </c>
@@ -11160,7 +11159,7 @@
       </c>
       <c r="L41" s="43">
         <f t="shared" si="29"/>
-        <v>67661</v>
+        <v>99775</v>
       </c>
       <c r="O41" s="80"/>
       <c r="P41" s="43">
@@ -11232,13 +11231,13 @@
         <v>3875190</v>
       </c>
     </row>
-    <row r="42" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:32" x14ac:dyDescent="0.3">
       <c r="O42" s="78" t="s">
         <v>143</v>
       </c>
       <c r="Y42" s="84"/>
     </row>
-    <row r="43" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B43" s="60" t="s">
         <v>142</v>
       </c>
@@ -11251,7 +11250,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B44" s="49" t="s">
         <v>51</v>
       </c>
@@ -11291,9 +11290,9 @@
         <f t="shared" si="39"/>
         <v>45016</v>
       </c>
-      <c r="L44" s="51" t="str">
+      <c r="L44" s="50">
         <f t="shared" si="39"/>
-        <v>31 กันยายน 2566</v>
+        <v>2566</v>
       </c>
       <c r="M44" s="86"/>
       <c r="O44" s="50">
@@ -11351,7 +11350,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="45" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B45" s="39" t="s">
         <v>42</v>
       </c>
@@ -11390,7 +11389,7 @@
       </c>
       <c r="L45" s="79">
         <f>IF(L27*J27=0,"",L27/J27-1)</f>
-        <v>3.6519079522283713</v>
+        <v>5.5353189630061168</v>
       </c>
       <c r="M45" s="90"/>
       <c r="O45" s="79"/>
@@ -11463,7 +11462,7 @@
         <v>0.18718932717571546</v>
       </c>
     </row>
-    <row r="46" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B46" s="41" t="s">
         <v>137</v>
       </c>
@@ -11502,7 +11501,7 @@
       </c>
       <c r="L46" s="79">
         <f t="shared" ref="L46:L50" si="43">IF(L28*J28=0,"",L28/J28-1)</f>
-        <v>1.506849315068493</v>
+        <v>2.8219178082191783</v>
       </c>
       <c r="M46" s="90"/>
       <c r="O46" s="79"/>
@@ -11575,7 +11574,7 @@
         <v>0.17918759473748147</v>
       </c>
     </row>
-    <row r="47" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B47" s="41" t="s">
         <v>138</v>
       </c>
@@ -11614,7 +11613,7 @@
       </c>
       <c r="L47" s="79">
         <f t="shared" si="43"/>
-        <v>0.93984035684939538</v>
+        <v>1.2955745979575068</v>
       </c>
       <c r="M47" s="90"/>
       <c r="O47" s="79"/>
@@ -11687,7 +11686,7 @@
         <v>0.18632609168066327</v>
       </c>
     </row>
-    <row r="48" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B48" s="39" t="s">
         <v>45</v>
       </c>
@@ -11726,7 +11725,7 @@
       </c>
       <c r="L48" s="79">
         <f t="shared" si="43"/>
-        <v>9.4230769230769234</v>
+        <v>10.653846153846153</v>
       </c>
       <c r="M48" s="90"/>
       <c r="O48" s="79"/>
@@ -11799,7 +11798,7 @@
         <v>0.17816381139611814</v>
       </c>
     </row>
-    <row r="49" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B49" s="39" t="s">
         <v>46</v>
       </c>
@@ -11838,7 +11837,7 @@
       </c>
       <c r="L49" s="79">
         <f t="shared" si="43"/>
-        <v>0.94471947194719474</v>
+        <v>0.9958745874587458</v>
       </c>
       <c r="M49" s="90"/>
       <c r="O49" s="79"/>
@@ -11911,7 +11910,7 @@
         <v>0.17372556281579854</v>
       </c>
     </row>
-    <row r="50" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B50" s="42" t="s">
         <v>47</v>
       </c>
@@ -11950,7 +11949,7 @@
       </c>
       <c r="L50" s="80">
         <f t="shared" si="43"/>
-        <v>2.1090676724541004</v>
+        <v>3.1100963186933077</v>
       </c>
       <c r="M50" s="90"/>
       <c r="O50" s="80"/>
@@ -12023,7 +12022,7 @@
         <v>0.18568370707514625</v>
       </c>
     </row>
-    <row r="51" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:32" x14ac:dyDescent="0.3">
       <c r="O51" s="81"/>
       <c r="P51" s="82"/>
       <c r="Q51" s="82"/>
@@ -12043,7 +12042,7 @@
       <c r="AE51" s="82"/>
       <c r="AF51" s="82"/>
     </row>
-    <row r="52" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B52" s="53" t="s">
         <v>52</v>
       </c>
@@ -12083,16 +12082,16 @@
         <f t="shared" si="53"/>
         <v>45016</v>
       </c>
-      <c r="L52" s="55" t="str">
+      <c r="L52" s="54">
         <f t="shared" si="53"/>
-        <v>31 กันยายน 2566</v>
+        <v>2566</v>
       </c>
       <c r="M52" s="55" t="s">
         <v>149</v>
       </c>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B53" s="39" t="s">
         <v>42</v>
       </c>
@@ -12134,14 +12133,14 @@
       </c>
       <c r="L53" s="40">
         <f t="shared" ref="L53" si="55">L22</f>
-        <v>13056852</v>
+        <v>13161395</v>
       </c>
       <c r="M53" s="79">
         <f>L53/L$58</f>
-        <v>0.29553811384835726</v>
-      </c>
-    </row>
-    <row r="54" spans="2:32" x14ac:dyDescent="0.35">
+        <v>0.2966685244052184</v>
+      </c>
+    </row>
+    <row r="54" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B54" s="41" t="s">
         <v>137</v>
       </c>
@@ -12183,14 +12182,14 @@
       </c>
       <c r="L54" s="40">
         <f t="shared" ref="L54" si="57">L19</f>
-        <v>7109198</v>
+        <v>7106524</v>
       </c>
       <c r="M54" s="79">
         <f t="shared" ref="M54:M57" si="58">L54/L$58</f>
-        <v>0.16091466518074293</v>
-      </c>
-    </row>
-    <row r="55" spans="2:32" x14ac:dyDescent="0.35">
+        <v>0.16018681824611072</v>
+      </c>
+    </row>
+    <row r="55" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B55" s="41" t="s">
         <v>138</v>
       </c>
@@ -12232,14 +12231,14 @@
       </c>
       <c r="L55" s="40">
         <f t="shared" ref="L55" si="60">SUM(L15:L18)</f>
-        <v>22643026</v>
+        <v>22719693</v>
       </c>
       <c r="M55" s="79">
         <f t="shared" si="58"/>
-        <v>0.512518422959785</v>
-      </c>
-    </row>
-    <row r="56" spans="2:32" x14ac:dyDescent="0.35">
+        <v>0.5121203183438815</v>
+      </c>
+    </row>
+    <row r="56" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B56" s="39" t="s">
         <v>45</v>
       </c>
@@ -12281,14 +12280,14 @@
       </c>
       <c r="L56" s="40">
         <f t="shared" ref="L56" si="62">L21</f>
-        <v>1241250</v>
+        <v>1247128</v>
       </c>
       <c r="M56" s="79">
         <f t="shared" si="58"/>
-        <v>2.8095339046063591E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="2:32" x14ac:dyDescent="0.35">
+        <v>2.8111277224369548E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B57" s="39" t="s">
         <v>46</v>
       </c>
@@ -12330,14 +12329,14 @@
       </c>
       <c r="L57" s="40">
         <f t="shared" ref="L57" si="64">L20</f>
-        <v>129600</v>
+        <v>129235</v>
       </c>
       <c r="M57" s="79">
         <f t="shared" si="58"/>
-        <v>2.9334589650512315E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="2:32" x14ac:dyDescent="0.35">
+        <v>2.9130617804198114E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B58" s="42" t="s">
         <v>47</v>
       </c>
@@ -12379,14 +12378,14 @@
       </c>
       <c r="L58" s="43">
         <f t="shared" ref="L58" si="66">SUM(L53:L57)</f>
-        <v>44179926</v>
+        <v>44363975</v>
       </c>
       <c r="M58" s="80">
         <f t="shared" ref="M58" si="67">K58/K$58</f>
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B60" s="64" t="s">
         <v>44</v>
       </c>
@@ -12426,13 +12425,13 @@
         <f t="shared" si="68"/>
         <v>45016</v>
       </c>
-      <c r="L60" s="66" t="str">
+      <c r="L60" s="65">
         <f t="shared" si="68"/>
-        <v>31 กันยายน 2566</v>
+        <v>2566</v>
       </c>
       <c r="M60" s="91"/>
     </row>
-    <row r="61" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B61" s="39" t="s">
         <v>42</v>
       </c>
@@ -12474,11 +12473,11 @@
       </c>
       <c r="L61" s="44">
         <f t="shared" ref="L61" si="70">L27/L53</f>
-        <v>4.8924503394845867E-3</v>
+        <v>6.8186541016358833E-3</v>
       </c>
       <c r="M61" s="92"/>
     </row>
-    <row r="62" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B62" s="41" t="s">
         <v>137</v>
       </c>
@@ -12520,11 +12519,11 @@
       </c>
       <c r="L62" s="44">
         <f t="shared" ref="L62" si="72">L28/L54</f>
-        <v>2.5741300214173243E-5</v>
+        <v>3.9259699960205579E-5</v>
       </c>
       <c r="M62" s="92"/>
     </row>
-    <row r="63" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B63" s="41" t="s">
         <v>138</v>
       </c>
@@ -12566,11 +12565,11 @@
       </c>
       <c r="L63" s="44">
         <f t="shared" ref="L63" si="74">L29/L55</f>
-        <v>1.4596547298934338E-3</v>
+        <v>1.7215021347339507E-3</v>
       </c>
       <c r="M63" s="92"/>
     </row>
-    <row r="64" spans="2:32" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B64" s="39" t="s">
         <v>45</v>
       </c>
@@ -12612,11 +12611,11 @@
       </c>
       <c r="L64" s="44">
         <f t="shared" ref="L64" si="76">L30/L56</f>
-        <v>2.1832829808660623E-4</v>
+        <v>2.4295822080812877E-4</v>
       </c>
       <c r="M64" s="92"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B65" s="39" t="s">
         <v>46</v>
       </c>
@@ -12658,11 +12657,11 @@
       </c>
       <c r="L65" s="44">
         <f t="shared" ref="L65" si="78">L31/L57</f>
-        <v>1.8186728395061729E-2</v>
+        <v>1.8717839594537083E-2</v>
       </c>
       <c r="M65" s="92"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B66" s="42" t="s">
         <v>47</v>
       </c>
@@ -12704,16 +12703,16 @@
       </c>
       <c r="L66" s="45">
         <f t="shared" ref="L66" si="80">L32/L58</f>
-        <v>2.2576316673776232E-3</v>
+        <v>2.972141247487404E-3</v>
       </c>
       <c r="M66" s="92"/>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B68" s="60" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B69" s="53" t="s">
         <v>52</v>
       </c>
@@ -12753,15 +12752,15 @@
         <f t="shared" si="81"/>
         <v>45016</v>
       </c>
-      <c r="L69" s="55" t="str">
+      <c r="L69" s="54">
         <f t="shared" si="81"/>
-        <v>31 กันยายน 2566</v>
+        <v>2566</v>
       </c>
       <c r="M69" s="55" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B70" s="39" t="s">
         <v>42</v>
       </c>
@@ -12803,11 +12802,11 @@
       </c>
       <c r="L70" s="40">
         <f t="shared" si="83"/>
-        <v>13056852</v>
+        <v>13161395</v>
       </c>
       <c r="M70" s="79"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B71" s="41" t="s">
         <v>137</v>
       </c>
@@ -12849,11 +12848,11 @@
       </c>
       <c r="L71" s="40">
         <f t="shared" si="85"/>
-        <v>7109198</v>
+        <v>7106524</v>
       </c>
       <c r="M71" s="79"/>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B72" s="41" t="s">
         <v>138</v>
       </c>
@@ -12895,11 +12894,11 @@
       </c>
       <c r="L72" s="40">
         <f t="shared" si="87"/>
-        <v>22643026</v>
+        <v>22719693</v>
       </c>
       <c r="M72" s="79"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B73" s="39" t="s">
         <v>45</v>
       </c>
@@ -12941,11 +12940,11 @@
       </c>
       <c r="L73" s="40">
         <f t="shared" si="89"/>
-        <v>1241250</v>
+        <v>1247128</v>
       </c>
       <c r="M73" s="79"/>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B74" s="39" t="s">
         <v>46</v>
       </c>
@@ -12987,11 +12986,11 @@
       </c>
       <c r="L74" s="40">
         <f t="shared" si="91"/>
-        <v>129600</v>
+        <v>129235</v>
       </c>
       <c r="M74" s="79"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B75" s="42" t="s">
         <v>47</v>
       </c>
@@ -13033,11 +13032,11 @@
       </c>
       <c r="L75" s="43">
         <f t="shared" si="93"/>
-        <v>44179926</v>
+        <v>44363975</v>
       </c>
       <c r="M75" s="80"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B77" s="59" t="s">
         <v>144</v>
       </c>
@@ -13046,7 +13045,7 @@
       </c>
       <c r="L77" s="77"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B78" s="53" t="s">
         <v>52</v>
       </c>
@@ -13086,12 +13085,12 @@
         <f>K44</f>
         <v>45016</v>
       </c>
-      <c r="L78" s="54" t="str">
+      <c r="L78" s="54">
         <f t="shared" si="94"/>
-        <v>31 กันยายน 2566</v>
-      </c>
-    </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.35">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B79" s="39" t="s">
         <v>42</v>
       </c>
@@ -13130,10 +13129,10 @@
       </c>
       <c r="L79" s="40">
         <f>L70-J70</f>
-        <v>407732</v>
-      </c>
-    </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.35">
+        <v>512275</v>
+      </c>
+    </row>
+    <row r="80" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B80" s="41" t="s">
         <v>137</v>
       </c>
@@ -13172,10 +13171,10 @@
       </c>
       <c r="L80" s="40">
         <f t="shared" ref="L80:L84" si="103">L71-J71</f>
-        <v>23288</v>
-      </c>
-    </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.35">
+        <v>20614</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B81" s="41" t="s">
         <v>138</v>
       </c>
@@ -13214,10 +13213,10 @@
       </c>
       <c r="L81" s="40">
         <f t="shared" si="103"/>
-        <v>342307</v>
-      </c>
-    </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.35">
+        <v>418974</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B82" s="39" t="s">
         <v>45</v>
       </c>
@@ -13256,10 +13255,10 @@
       </c>
       <c r="L82" s="40">
         <f t="shared" si="103"/>
-        <v>15701</v>
-      </c>
-    </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.35">
+        <v>21579</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B83" s="39" t="s">
         <v>46</v>
       </c>
@@ -13298,10 +13297,10 @@
       </c>
       <c r="L83" s="40">
         <f t="shared" si="103"/>
-        <v>-3206</v>
-      </c>
-    </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.35">
+        <v>-3571</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B84" s="42" t="s">
         <v>47</v>
       </c>
@@ -13340,10 +13339,10 @@
       </c>
       <c r="L84" s="43">
         <f t="shared" si="103"/>
-        <v>785822</v>
-      </c>
-    </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.35">
+        <v>969871</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B86" s="60" t="s">
         <v>142</v>
       </c>
@@ -13352,7 +13351,7 @@
       </c>
       <c r="L86" s="77"/>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B87" s="53" t="s">
         <v>52</v>
       </c>
@@ -13392,12 +13391,12 @@
         <f t="shared" si="104"/>
         <v>45016</v>
       </c>
-      <c r="L87" s="54" t="str">
+      <c r="L87" s="54">
         <f t="shared" si="104"/>
-        <v>31 กันยายน 2566</v>
-      </c>
-    </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.35">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B88" s="39" t="s">
         <v>42</v>
       </c>
@@ -13436,10 +13435,10 @@
       </c>
       <c r="L88" s="79">
         <f>IF(L70*J70=0,"",L70/J70-1)</f>
-        <v>3.2234021022806258E-2</v>
-      </c>
-    </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.35">
+        <v>4.049886474315989E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B89" s="41" t="s">
         <v>137</v>
       </c>
@@ -13478,10 +13477,10 @@
       </c>
       <c r="L89" s="79">
         <f t="shared" ref="L89:L93" si="113">IF(L71*J71=0,"",L71/J71-1)</f>
-        <v>3.2865221263040922E-3</v>
-      </c>
-    </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.35">
+        <v>2.9091535173322303E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B90" s="41" t="s">
         <v>138</v>
       </c>
@@ -13520,10 +13519,10 @@
       </c>
       <c r="L90" s="79">
         <f t="shared" si="113"/>
-        <v>1.5349594782123388E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.35">
+        <v>1.8787466000535602E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B91" s="39" t="s">
         <v>45</v>
       </c>
@@ -13562,10 +13561,10 @@
       </c>
       <c r="L91" s="79">
         <f t="shared" si="113"/>
-        <v>1.2811401257722066E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.35">
+        <v>1.7607619116004392E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B92" s="39" t="s">
         <v>46</v>
       </c>
@@ -13604,10 +13603,10 @@
       </c>
       <c r="L92" s="79">
         <f t="shared" si="113"/>
-        <v>-2.4140475580922582E-2</v>
-      </c>
-    </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.35">
+        <v>-2.6888845383491677E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B93" s="42" t="s">
         <v>47</v>
       </c>
@@ -13646,10 +13645,10 @@
       </c>
       <c r="L93" s="80">
         <f t="shared" si="113"/>
-        <v>1.8108957843673945E-2</v>
-      </c>
-    </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.35">
+        <v>2.2350294408659765E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B95" s="64" t="s">
         <v>150</v>
       </c>
@@ -13689,12 +13688,12 @@
         <f>K44</f>
         <v>45016</v>
       </c>
-      <c r="L95" s="66" t="str">
+      <c r="L95" s="65">
         <f t="shared" ref="L95" si="115">L44</f>
-        <v>31 กันยายน 2566</v>
-      </c>
-    </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.35">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B96" s="39" t="s">
         <v>42</v>
       </c>
@@ -13733,10 +13732,10 @@
       </c>
       <c r="L96" s="44">
         <f>L36/L79</f>
-        <v>0.12299255393248507</v>
-      </c>
-    </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0.14837928846810794</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B97" s="41" t="s">
         <v>137</v>
       </c>
@@ -13775,10 +13774,10 @@
       </c>
       <c r="L97" s="44">
         <f t="shared" ref="L97:L101" si="117">L37/L80</f>
-        <v>4.7234627275850221E-3</v>
-      </c>
-    </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.35">
+        <v>9.993208499078296E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B98" s="41" t="s">
         <v>138</v>
       </c>
@@ -13817,10 +13816,10 @@
       </c>
       <c r="L98" s="44">
         <f t="shared" si="117"/>
-        <v>4.677964517231608E-2</v>
-      </c>
-    </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.35">
+        <v>5.2685846854458748E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B99" s="39" t="s">
         <v>45</v>
       </c>
@@ -13859,10 +13858,10 @@
       </c>
       <c r="L99" s="44">
         <f t="shared" si="117"/>
-        <v>1.5604101649576461E-2</v>
-      </c>
-    </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.35">
+        <v>1.2836554057185227E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B100" s="39" t="s">
         <v>46</v>
       </c>
@@ -13901,10 +13900,10 @@
       </c>
       <c r="L100" s="44">
         <f t="shared" si="117"/>
-        <v>-0.35714285714285715</v>
-      </c>
-    </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.35">
+        <v>-0.33800056006720808</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B101" s="42" t="s">
         <v>47</v>
       </c>
@@ -13943,7 +13942,7 @@
       </c>
       <c r="L101" s="45">
         <f t="shared" si="117"/>
-        <v>8.6102196171652101E-2</v>
+        <v>0.10287450599100292</v>
       </c>
     </row>
   </sheetData>
@@ -13961,18 +13960,18 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="67"/>
-    <col min="2" max="2" width="4.8984375" style="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.875" style="67" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" style="67" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.8984375" style="67" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.09765625" style="67" customWidth="1"/>
-    <col min="6" max="6" width="48.09765625" style="67" customWidth="1"/>
+    <col min="4" max="4" width="73.875" style="67" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.125" style="67" customWidth="1"/>
+    <col min="6" max="6" width="48.125" style="67" customWidth="1"/>
     <col min="7" max="16384" width="9" style="67"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="70" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C2" s="70" t="s">
         <v>85</v>
       </c>
@@ -13986,7 +13985,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="B3" s="67">
         <v>2553</v>
       </c>
@@ -13998,7 +13997,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="99.75" x14ac:dyDescent="0.2">
       <c r="B4" s="67">
         <f>C4+543</f>
         <v>2558</v>
@@ -14010,7 +14009,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="110.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="114" x14ac:dyDescent="0.2">
       <c r="B5" s="67">
         <f t="shared" ref="B5:B12" si="0">C5+543</f>
         <v>2559</v>
@@ -14025,7 +14024,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="57" x14ac:dyDescent="0.2">
       <c r="B6" s="67">
         <f t="shared" si="0"/>
         <v>2560</v>
@@ -14038,7 +14037,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B7" s="67">
         <f t="shared" si="0"/>
         <v>2561</v>
@@ -14053,7 +14052,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="215.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="215.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="67">
         <f t="shared" si="0"/>
         <v>2562</v>
@@ -14068,7 +14067,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="317.39999999999998" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="327.75" x14ac:dyDescent="0.2">
       <c r="B9" s="67">
         <f t="shared" si="0"/>
         <v>2563</v>
@@ -14083,7 +14082,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B10" s="67">
         <f t="shared" si="0"/>
         <v>2564</v>
@@ -14101,7 +14100,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B11" s="67">
         <f t="shared" si="0"/>
         <v>2565</v>
@@ -14119,7 +14118,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="138" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="156.75" x14ac:dyDescent="0.2">
       <c r="B12" s="67">
         <f t="shared" si="0"/>
         <v>2566</v>
@@ -14148,28 +14147,28 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="7.5" style="74" customWidth="1"/>
     <col min="3" max="3" width="94" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B1" s="74" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="74" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="74" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="74">
         <v>2018</v>
       </c>
@@ -14177,7 +14176,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="74">
         <v>2019</v>
       </c>
@@ -14185,22 +14184,22 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="74" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="74" t="s">
         <v>114</v>
       </c>
@@ -14208,17 +14207,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>123</v>
       </c>
@@ -14226,74 +14225,74 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="74" t="s">
         <v>124</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" s="74" t="s">
         <v>125</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" s="74" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" s="74" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>133</v>
       </c>

</xml_diff>

<commit_message>
update data and add dashboard
</commit_message>
<xml_diff>
--- a/rawdata/01 EGAT_EV_เตรียมข้อมูลประชุม_Sep2023.xlsx
+++ b/rawdata/01 EGAT_EV_เตรียมข้อมูลประชุม_Sep2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rstudio\thailandVehicleAnalysis\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015E09AC-0DC6-4FEC-9BD1-3E17F08B92AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0FACA1-E52C-49E8-98E1-39B58FAF4AAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="2" activeTab="2" xr2:uid="{EDD8F08D-6CA6-4516-B97F-8A475C3F3159}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="9060" firstSheet="2" activeTab="2" xr2:uid="{EDD8F08D-6CA6-4516-B97F-8A475C3F3159}"/>
   </bookViews>
   <sheets>
     <sheet name="M2_Ques_Sep22" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="M3_Timeline" sheetId="4" r:id="rId4"/>
     <sheet name="M3_สรุปโครงการ" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -321,7 +321,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -331,7 +331,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -345,7 +345,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -355,7 +355,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -388,7 +388,7 @@
         <u/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -398,7 +398,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -415,7 +415,7 @@
         <u/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -425,7 +425,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -441,7 +441,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -451,7 +451,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -463,7 +463,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -473,7 +473,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -490,7 +490,7 @@
         <u/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -500,7 +500,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -511,7 +511,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -521,7 +521,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -533,7 +533,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -543,7 +543,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -555,7 +555,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -565,7 +565,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -577,7 +577,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -587,7 +587,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -600,7 +600,7 @@
         <u/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -610,7 +610,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -626,7 +626,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -637,7 +637,7 @@
         <u/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -647,7 +647,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -657,7 +657,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -670,7 +670,7 @@
         <u/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -680,7 +680,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -693,7 +693,7 @@
         <u/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -703,7 +703,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -729,7 +729,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -739,7 +739,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -751,7 +751,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -761,7 +761,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -775,7 +775,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -785,7 +785,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -813,7 +813,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -823,7 +823,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -842,7 +842,7 @@
         <u/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -852,7 +852,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -862,7 +862,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -873,7 +873,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -883,7 +883,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -1008,17 +1008,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="187" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="188" formatCode="B1mmm\-yy"/>
-    <numFmt numFmtId="189" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="190" formatCode="[$-107041E]d\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="191" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="B1mmm\-yy"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="[$-107041E]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -1026,14 +1026,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -1042,7 +1049,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1062,7 +1069,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -1078,7 +1085,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="major"/>
@@ -1096,14 +1103,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1111,13 +1118,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1125,7 +1132,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1133,7 +1140,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1141,7 +1148,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -1305,9 +1312,9 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1317,19 +1324,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="188" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1338,83 +1345,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="4" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="191" fontId="5" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="191" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="190" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="190" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="7" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="190" fontId="7" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1426,55 +1433,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="189" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="190" fontId="7" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="189" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="190" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="6" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="190" fontId="7" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="8" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="191" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2093,7 +2100,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="th-TH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1934495967"/>
@@ -2152,7 +2159,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="th-TH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1873548687"/>
@@ -2200,7 +2207,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="th-TH"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2804,7 +2811,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="th-TH"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2842,7 +2849,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="th-TH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1943285007"/>
@@ -2922,7 +2929,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="th-TH"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2960,7 +2967,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="th-TH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1934291791"/>
@@ -3012,7 +3019,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="th-TH"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3049,7 +3056,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="th-TH"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3126,7 +3133,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="th-TH"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3709,7 +3716,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="th-TH"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3747,7 +3754,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="th-TH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1943285007"/>
@@ -3827,7 +3834,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="th-TH"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3865,7 +3872,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="th-TH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1934291791"/>
@@ -3907,7 +3914,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="th-TH"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3944,7 +3951,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="th-TH"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3995,7 +4002,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="th-TH"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4675,7 +4682,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="th-TH"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4713,7 +4720,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="th-TH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1943285007"/>
@@ -4793,7 +4800,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="th-TH"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4831,7 +4838,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="th-TH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1934291791"/>
@@ -4879,7 +4886,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="th-TH"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7297,7 +7304,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>513504</xdr:colOff>
+      <xdr:colOff>226634</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>4705</xdr:rowOff>
     </xdr:to>
@@ -7341,7 +7348,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>468405</xdr:colOff>
+      <xdr:colOff>181534</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>67236</xdr:rowOff>
     </xdr:to>
@@ -7371,13 +7378,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>470645</xdr:colOff>
+      <xdr:colOff>183774</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>134470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>134471</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>466165</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>80682</xdr:rowOff>
     </xdr:to>
@@ -7406,14 +7413,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>206189</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>537883</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>125505</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>89648</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>475130</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>71717</xdr:rowOff>
     </xdr:to>
@@ -7442,14 +7449,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>143437</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>528919</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>116541</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>62753</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>376518</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>62753</xdr:rowOff>
     </xdr:to>
@@ -7832,164 +7839,164 @@
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2">
       <c r="B2" s="61" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2">
       <c r="B3" s="62" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2">
       <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2">
       <c r="B5" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2">
       <c r="B6" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2">
       <c r="B7" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:2">
       <c r="B8" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:2">
       <c r="B9" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:2">
       <c r="B10" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:2">
       <c r="B11" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:2">
       <c r="B12" s="63" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:2">
       <c r="B14" s="62" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:2">
       <c r="B15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:2">
       <c r="B16" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2">
       <c r="B18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2">
       <c r="B19" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2">
       <c r="B20" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2">
       <c r="B21" s="63" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2">
       <c r="B22" s="63" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2">
       <c r="B23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2">
       <c r="B24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2">
       <c r="B25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:2">
       <c r="B26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2">
       <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:2">
       <c r="B28" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2">
       <c r="B29" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2">
       <c r="B30" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2">
       <c r="B31" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2">
       <c r="B32" s="63" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2">
       <c r="B33" s="63" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2">
       <c r="B34" s="1" t="s">
         <v>84</v>
       </c>
@@ -8008,20 +8015,20 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:15">
       <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
@@ -8062,7 +8069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:15">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
@@ -8104,7 +8111,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:15">
       <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
@@ -8150,7 +8157,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:15">
       <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
@@ -8196,7 +8203,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:15">
       <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
@@ -8242,7 +8249,7 @@
         <v>0.20340501792114685</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:15">
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
@@ -8250,7 +8257,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:15">
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -8259,7 +8266,7 @@
         <v>1.2034050179211468</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:15">
       <c r="B10" s="15" t="s">
         <v>24</v>
       </c>
@@ -8279,7 +8286,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15">
       <c r="B11" s="16" t="s">
         <v>19</v>
       </c>
@@ -8299,7 +8306,7 @@
         <v>7325</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15">
       <c r="B12" s="17" t="s">
         <v>20</v>
       </c>
@@ -8319,7 +8326,7 @@
         <v>5947</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:15">
       <c r="B13" s="11" t="s">
         <v>21</v>
       </c>
@@ -8339,7 +8346,7 @@
         <v>32718</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:15">
       <c r="B14" s="11" t="s">
         <v>22</v>
       </c>
@@ -8359,7 +8366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15" s="18" customFormat="1">
       <c r="B15" s="19" t="s">
         <v>23</v>
       </c>
@@ -8384,7 +8391,7 @@
         <v>45990</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11">
       <c r="B17" s="15" t="s">
         <v>25</v>
       </c>
@@ -8404,7 +8411,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11">
       <c r="B18" s="16" t="s">
         <v>19</v>
       </c>
@@ -8431,7 +8438,7 @@
         <v>21.805847953216375</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11">
       <c r="B19" s="17" t="s">
         <v>20</v>
       </c>
@@ -8447,7 +8454,7 @@
         <v>37075</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11">
       <c r="B20" s="11" t="s">
         <v>21</v>
       </c>
@@ -8463,7 +8470,7 @@
         <v>228894</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11">
       <c r="B21" s="11" t="s">
         <v>22</v>
       </c>
@@ -8477,7 +8484,7 @@
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11">
       <c r="B22" s="19" t="s">
         <v>23</v>
       </c>
@@ -8502,7 +8509,7 @@
         <v>284613</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11">
       <c r="B24" s="13" t="s">
         <v>31</v>
       </c>
@@ -8519,7 +8526,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11">
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
@@ -8537,7 +8544,7 @@
         <v>264361</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11">
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
@@ -8555,7 +8562,7 @@
         <v>19570</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11">
       <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
@@ -8573,7 +8580,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11">
       <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
@@ -8591,7 +8598,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11">
       <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
@@ -8609,7 +8616,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11">
       <c r="B30" s="5" t="s">
         <v>32</v>
       </c>
@@ -8646,37 +8653,37 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-      <selection pane="bottomRight" activeCell="L36" sqref="L36"/>
+      <selection pane="bottomRight" activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="8.75" style="32"/>
-    <col min="2" max="2" width="22.875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="12.75" style="31" customWidth="1"/>
-    <col min="4" max="10" width="12.625" style="31" customWidth="1"/>
-    <col min="11" max="11" width="13.5" style="31" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.25" style="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="32"/>
+    <col min="2" max="2" width="22.88671875" style="30" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="31" customWidth="1"/>
+    <col min="4" max="10" width="12.6640625" style="31" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="31" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.21875" style="31" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" style="31" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="8.75" style="32"/>
-    <col min="16" max="16" width="8" style="32" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.875" style="32" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8" style="32" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.77734375" style="32"/>
+    <col min="16" max="16" width="9.77734375" style="32" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="32" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="32" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="32" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" style="32" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.875" style="32" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="8.75" style="32" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.88671875" style="32" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="8.77734375" style="32" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="9" style="32" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.875" style="32" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.125" style="32" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.875" style="32" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="9.75" style="32" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.875" style="32" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.25" style="32" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.75" style="32"/>
+    <col min="26" max="26" width="8.88671875" style="32" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.88671875" style="32" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="9.77734375" style="32" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.88671875" style="32" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.21875" style="32" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="8.77734375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:32">
       <c r="B1" s="59" t="s">
         <v>49</v>
       </c>
@@ -8689,7 +8696,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="2:32" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:32" s="48" customFormat="1">
       <c r="B2" s="49" t="s">
         <v>51</v>
       </c>
@@ -8701,7 +8708,7 @@
         <v>2559</v>
       </c>
       <c r="E2" s="50">
-        <f t="shared" ref="E2:L2" si="0">D2+1</f>
+        <f t="shared" ref="E2:J2" si="0">D2+1</f>
         <v>2560</v>
       </c>
       <c r="F2" s="50">
@@ -8786,7 +8793,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="3" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:32">
       <c r="B3" s="34" t="s">
         <v>38</v>
       </c>
@@ -8840,7 +8847,7 @@
       <c r="AE3" s="35"/>
       <c r="AF3" s="35"/>
     </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:32">
       <c r="B4" s="34" t="s">
         <v>39</v>
       </c>
@@ -8894,7 +8901,7 @@
       <c r="AE4" s="35"/>
       <c r="AF4" s="35"/>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:32">
       <c r="B5" s="34" t="s">
         <v>36</v>
       </c>
@@ -8948,7 +8955,7 @@
       <c r="AE5" s="35"/>
       <c r="AF5" s="35"/>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:32">
       <c r="B6" s="34" t="s">
         <v>37</v>
       </c>
@@ -9002,7 +9009,7 @@
       <c r="AE6" s="35"/>
       <c r="AF6" s="35"/>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:32">
       <c r="B7" s="76" t="s">
         <v>136</v>
       </c>
@@ -9056,7 +9063,7 @@
       <c r="AE7" s="35"/>
       <c r="AF7" s="35"/>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:32">
       <c r="B8" s="76" t="s">
         <v>135</v>
       </c>
@@ -9110,7 +9117,7 @@
       <c r="AE8" s="35"/>
       <c r="AF8" s="35"/>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:32">
       <c r="B9" s="76" t="s">
         <v>134</v>
       </c>
@@ -9164,7 +9171,7 @@
       <c r="AE9" s="35"/>
       <c r="AF9" s="35"/>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:32">
       <c r="B10" s="75" t="s">
         <v>42</v>
       </c>
@@ -9228,7 +9235,7 @@
       <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
     </row>
-    <row r="11" spans="2:32" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:32" s="33" customFormat="1">
       <c r="B11" s="37" t="s">
         <v>35</v>
       </c>
@@ -9282,7 +9289,7 @@
       <c r="AE11" s="38"/>
       <c r="AF11" s="38"/>
     </row>
-    <row r="12" spans="2:32" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:32" s="33" customFormat="1">
       <c r="B12" s="46" t="s">
         <v>48</v>
       </c>
@@ -9298,7 +9305,7 @@
       <c r="L12" s="47"/>
       <c r="M12" s="47"/>
     </row>
-    <row r="14" spans="2:32" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:32" s="52" customFormat="1">
       <c r="B14" s="53" t="s">
         <v>52</v>
       </c>
@@ -9344,7 +9351,7 @@
       </c>
       <c r="M14" s="89"/>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:32">
       <c r="B15" s="34" t="s">
         <v>38</v>
       </c>
@@ -9380,7 +9387,7 @@
       </c>
       <c r="M15" s="87"/>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:32">
       <c r="B16" s="34" t="s">
         <v>39</v>
       </c>
@@ -9416,7 +9423,7 @@
       </c>
       <c r="M16" s="87"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32">
       <c r="B17" s="34" t="s">
         <v>36</v>
       </c>
@@ -9452,7 +9459,7 @@
       </c>
       <c r="M17" s="87"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32">
       <c r="B18" s="34" t="s">
         <v>37</v>
       </c>
@@ -9488,7 +9495,7 @@
       </c>
       <c r="M18" s="87"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32">
       <c r="B19" s="76" t="s">
         <v>136</v>
       </c>
@@ -9524,7 +9531,7 @@
       </c>
       <c r="M19" s="87"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32">
       <c r="B20" s="34" t="s">
         <v>40</v>
       </c>
@@ -9560,7 +9567,7 @@
       </c>
       <c r="M20" s="87"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32">
       <c r="B21" s="34" t="s">
         <v>41</v>
       </c>
@@ -9596,7 +9603,7 @@
       </c>
       <c r="M21" s="87"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32">
       <c r="B22" s="75" t="s">
         <v>42</v>
       </c>
@@ -9642,7 +9649,7 @@
       </c>
       <c r="M22" s="88"/>
     </row>
-    <row r="23" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" s="33" customFormat="1">
       <c r="B23" s="37" t="s">
         <v>43</v>
       </c>
@@ -9678,7 +9685,7 @@
       </c>
       <c r="M23" s="47"/>
     </row>
-    <row r="24" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" s="33" customFormat="1">
       <c r="A24" s="56"/>
       <c r="B24" s="57"/>
       <c r="C24" s="58"/>
@@ -9696,7 +9703,7 @@
       <c r="O24" s="56"/>
       <c r="P24" s="56"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32">
       <c r="B25" s="60" t="s">
         <v>50</v>
       </c>
@@ -9709,7 +9716,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32">
       <c r="B26" s="49" t="s">
         <v>51</v>
       </c>
@@ -9811,7 +9818,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32">
       <c r="B27" s="39" t="s">
         <v>42</v>
       </c>
@@ -9914,7 +9921,7 @@
         <v>7216379</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32">
       <c r="B28" s="41" t="s">
         <v>137</v>
       </c>
@@ -10017,7 +10024,7 @@
         <v>2232662</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32">
       <c r="B29" s="41" t="s">
         <v>138</v>
       </c>
@@ -10120,7 +10127,7 @@
         <v>14603170</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:32">
       <c r="B30" s="39" t="s">
         <v>45</v>
       </c>
@@ -10223,7 +10230,7 @@
         <v>604087</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32">
       <c r="B31" s="39" t="s">
         <v>46</v>
       </c>
@@ -10326,7 +10333,7 @@
         <v>88736</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32">
       <c r="B32" s="42" t="s">
         <v>47</v>
       </c>
@@ -10447,12 +10454,12 @@
         <v>24745034</v>
       </c>
     </row>
-    <row r="33" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:32">
       <c r="O33" s="78" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:32">
       <c r="B34" s="59" t="s">
         <v>144</v>
       </c>
@@ -10465,7 +10472,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:32">
       <c r="B35" s="49" t="s">
         <v>51</v>
       </c>
@@ -10565,7 +10572,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="36" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:32">
       <c r="B36" s="39" t="s">
         <v>42</v>
       </c>
@@ -10676,7 +10683,7 @@
         <v>1137838</v>
       </c>
     </row>
-    <row r="37" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:32">
       <c r="B37" s="41" t="s">
         <v>137</v>
       </c>
@@ -10787,7 +10794,7 @@
         <v>339272</v>
       </c>
     </row>
-    <row r="38" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:32">
       <c r="B38" s="41" t="s">
         <v>138</v>
       </c>
@@ -10898,7 +10905,7 @@
         <v>2293595</v>
       </c>
     </row>
-    <row r="39" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:32">
       <c r="B39" s="39" t="s">
         <v>45</v>
       </c>
@@ -11009,7 +11016,7 @@
         <v>91351</v>
       </c>
     </row>
-    <row r="40" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:32">
       <c r="B40" s="39" t="s">
         <v>46</v>
       </c>
@@ -11120,7 +11127,7 @@
         <v>13134</v>
       </c>
     </row>
-    <row r="41" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:32">
       <c r="B41" s="42" t="s">
         <v>47</v>
       </c>
@@ -11231,13 +11238,13 @@
         <v>3875190</v>
       </c>
     </row>
-    <row r="42" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:32">
       <c r="O42" s="78" t="s">
         <v>143</v>
       </c>
       <c r="Y42" s="84"/>
     </row>
-    <row r="43" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:32">
       <c r="B43" s="60" t="s">
         <v>142</v>
       </c>
@@ -11250,7 +11257,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:32">
       <c r="B44" s="49" t="s">
         <v>51</v>
       </c>
@@ -11350,7 +11357,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="45" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:32">
       <c r="B45" s="39" t="s">
         <v>42</v>
       </c>
@@ -11462,7 +11469,7 @@
         <v>0.18718932717571546</v>
       </c>
     </row>
-    <row r="46" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:32">
       <c r="B46" s="41" t="s">
         <v>137</v>
       </c>
@@ -11574,7 +11581,7 @@
         <v>0.17918759473748147</v>
       </c>
     </row>
-    <row r="47" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:32">
       <c r="B47" s="41" t="s">
         <v>138</v>
       </c>
@@ -11686,7 +11693,7 @@
         <v>0.18632609168066327</v>
       </c>
     </row>
-    <row r="48" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:32">
       <c r="B48" s="39" t="s">
         <v>45</v>
       </c>
@@ -11798,7 +11805,7 @@
         <v>0.17816381139611814</v>
       </c>
     </row>
-    <row r="49" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:32">
       <c r="B49" s="39" t="s">
         <v>46</v>
       </c>
@@ -11910,7 +11917,7 @@
         <v>0.17372556281579854</v>
       </c>
     </row>
-    <row r="50" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:32">
       <c r="B50" s="42" t="s">
         <v>47</v>
       </c>
@@ -12022,7 +12029,7 @@
         <v>0.18568370707514625</v>
       </c>
     </row>
-    <row r="51" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:32">
       <c r="O51" s="81"/>
       <c r="P51" s="82"/>
       <c r="Q51" s="82"/>
@@ -12042,7 +12049,7 @@
       <c r="AE51" s="82"/>
       <c r="AF51" s="82"/>
     </row>
-    <row r="52" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:32">
       <c r="B52" s="53" t="s">
         <v>52</v>
       </c>
@@ -12091,7 +12098,7 @@
       </c>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:32">
       <c r="B53" s="39" t="s">
         <v>42</v>
       </c>
@@ -12140,7 +12147,7 @@
         <v>0.2966685244052184</v>
       </c>
     </row>
-    <row r="54" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:32">
       <c r="B54" s="41" t="s">
         <v>137</v>
       </c>
@@ -12189,7 +12196,7 @@
         <v>0.16018681824611072</v>
       </c>
     </row>
-    <row r="55" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:32">
       <c r="B55" s="41" t="s">
         <v>138</v>
       </c>
@@ -12238,7 +12245,7 @@
         <v>0.5121203183438815</v>
       </c>
     </row>
-    <row r="56" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:32">
       <c r="B56" s="39" t="s">
         <v>45</v>
       </c>
@@ -12287,7 +12294,7 @@
         <v>2.8111277224369548E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:32">
       <c r="B57" s="39" t="s">
         <v>46</v>
       </c>
@@ -12336,7 +12343,7 @@
         <v>2.9130617804198114E-3</v>
       </c>
     </row>
-    <row r="58" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:32">
       <c r="B58" s="42" t="s">
         <v>47</v>
       </c>
@@ -12385,7 +12392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:32">
       <c r="B60" s="64" t="s">
         <v>44</v>
       </c>
@@ -12431,7 +12438,7 @@
       </c>
       <c r="M60" s="91"/>
     </row>
-    <row r="61" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:32">
       <c r="B61" s="39" t="s">
         <v>42</v>
       </c>
@@ -12477,7 +12484,7 @@
       </c>
       <c r="M61" s="92"/>
     </row>
-    <row r="62" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:32">
       <c r="B62" s="41" t="s">
         <v>137</v>
       </c>
@@ -12523,7 +12530,7 @@
       </c>
       <c r="M62" s="92"/>
     </row>
-    <row r="63" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:32">
       <c r="B63" s="41" t="s">
         <v>138</v>
       </c>
@@ -12569,7 +12576,7 @@
       </c>
       <c r="M63" s="92"/>
     </row>
-    <row r="64" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:32">
       <c r="B64" s="39" t="s">
         <v>45</v>
       </c>
@@ -12615,7 +12622,7 @@
       </c>
       <c r="M64" s="92"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:13">
       <c r="B65" s="39" t="s">
         <v>46</v>
       </c>
@@ -12661,7 +12668,7 @@
       </c>
       <c r="M65" s="92"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:13">
       <c r="B66" s="42" t="s">
         <v>47</v>
       </c>
@@ -12707,12 +12714,12 @@
       </c>
       <c r="M66" s="92"/>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:13">
       <c r="B68" s="60" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:13">
       <c r="B69" s="53" t="s">
         <v>52</v>
       </c>
@@ -12760,7 +12767,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:13">
       <c r="B70" s="39" t="s">
         <v>42</v>
       </c>
@@ -12806,7 +12813,7 @@
       </c>
       <c r="M70" s="79"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:13">
       <c r="B71" s="41" t="s">
         <v>137</v>
       </c>
@@ -12852,7 +12859,7 @@
       </c>
       <c r="M71" s="79"/>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:13">
       <c r="B72" s="41" t="s">
         <v>138</v>
       </c>
@@ -12898,7 +12905,7 @@
       </c>
       <c r="M72" s="79"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:13">
       <c r="B73" s="39" t="s">
         <v>45</v>
       </c>
@@ -12944,7 +12951,7 @@
       </c>
       <c r="M73" s="79"/>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:13">
       <c r="B74" s="39" t="s">
         <v>46</v>
       </c>
@@ -12990,7 +12997,7 @@
       </c>
       <c r="M74" s="79"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:13">
       <c r="B75" s="42" t="s">
         <v>47</v>
       </c>
@@ -13036,7 +13043,7 @@
       </c>
       <c r="M75" s="80"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:13">
       <c r="B77" s="59" t="s">
         <v>144</v>
       </c>
@@ -13045,7 +13052,7 @@
       </c>
       <c r="L77" s="77"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:13">
       <c r="B78" s="53" t="s">
         <v>52</v>
       </c>
@@ -13090,7 +13097,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:13">
       <c r="B79" s="39" t="s">
         <v>42</v>
       </c>
@@ -13132,7 +13139,7 @@
         <v>512275</v>
       </c>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:13">
       <c r="B80" s="41" t="s">
         <v>137</v>
       </c>
@@ -13174,7 +13181,7 @@
         <v>20614</v>
       </c>
     </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:12">
       <c r="B81" s="41" t="s">
         <v>138</v>
       </c>
@@ -13216,7 +13223,7 @@
         <v>418974</v>
       </c>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:12">
       <c r="B82" s="39" t="s">
         <v>45</v>
       </c>
@@ -13258,7 +13265,7 @@
         <v>21579</v>
       </c>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:12">
       <c r="B83" s="39" t="s">
         <v>46</v>
       </c>
@@ -13300,7 +13307,7 @@
         <v>-3571</v>
       </c>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:12">
       <c r="B84" s="42" t="s">
         <v>47</v>
       </c>
@@ -13342,7 +13349,7 @@
         <v>969871</v>
       </c>
     </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:12">
       <c r="B86" s="60" t="s">
         <v>142</v>
       </c>
@@ -13351,7 +13358,7 @@
       </c>
       <c r="L86" s="77"/>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:12">
       <c r="B87" s="53" t="s">
         <v>52</v>
       </c>
@@ -13396,7 +13403,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:12">
       <c r="B88" s="39" t="s">
         <v>42</v>
       </c>
@@ -13438,7 +13445,7 @@
         <v>4.049886474315989E-2</v>
       </c>
     </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:12">
       <c r="B89" s="41" t="s">
         <v>137</v>
       </c>
@@ -13480,7 +13487,7 @@
         <v>2.9091535173322303E-3</v>
       </c>
     </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:12">
       <c r="B90" s="41" t="s">
         <v>138</v>
       </c>
@@ -13522,7 +13529,7 @@
         <v>1.8787466000535602E-2</v>
       </c>
     </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:12">
       <c r="B91" s="39" t="s">
         <v>45</v>
       </c>
@@ -13564,7 +13571,7 @@
         <v>1.7607619116004392E-2</v>
       </c>
     </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:12">
       <c r="B92" s="39" t="s">
         <v>46</v>
       </c>
@@ -13606,7 +13613,7 @@
         <v>-2.6888845383491677E-2</v>
       </c>
     </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:12">
       <c r="B93" s="42" t="s">
         <v>47</v>
       </c>
@@ -13648,7 +13655,7 @@
         <v>2.2350294408659765E-2</v>
       </c>
     </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:12">
       <c r="B95" s="64" t="s">
         <v>150</v>
       </c>
@@ -13693,7 +13700,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:12">
       <c r="B96" s="39" t="s">
         <v>42</v>
       </c>
@@ -13735,7 +13742,7 @@
         <v>0.14837928846810794</v>
       </c>
     </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:12">
       <c r="B97" s="41" t="s">
         <v>137</v>
       </c>
@@ -13777,7 +13784,7 @@
         <v>9.993208499078296E-3</v>
       </c>
     </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:12">
       <c r="B98" s="41" t="s">
         <v>138</v>
       </c>
@@ -13819,7 +13826,7 @@
         <v>5.2685846854458748E-2</v>
       </c>
     </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:12">
       <c r="B99" s="39" t="s">
         <v>45</v>
       </c>
@@ -13861,7 +13868,7 @@
         <v>1.2836554057185227E-2</v>
       </c>
     </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:12">
       <c r="B100" s="39" t="s">
         <v>46</v>
       </c>
@@ -13903,7 +13910,7 @@
         <v>-0.33800056006720808</v>
       </c>
     </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:12">
       <c r="B101" s="42" t="s">
         <v>47</v>
       </c>
@@ -13960,18 +13967,18 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" style="67"/>
-    <col min="2" max="2" width="4.875" style="67" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" style="67" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.875" style="67" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.125" style="67" customWidth="1"/>
-    <col min="6" max="6" width="48.125" style="67" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" style="67" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" style="67" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.88671875" style="67" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.109375" style="67" customWidth="1"/>
+    <col min="6" max="6" width="48.109375" style="67" customWidth="1"/>
     <col min="7" max="16384" width="9" style="67"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="70" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" s="70" customFormat="1">
       <c r="C2" s="70" t="s">
         <v>85</v>
       </c>
@@ -13985,7 +13992,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" ht="100.8">
       <c r="B3" s="67">
         <v>2553</v>
       </c>
@@ -13997,7 +14004,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" ht="100.8">
       <c r="B4" s="67">
         <f>C4+543</f>
         <v>2558</v>
@@ -14009,7 +14016,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="114" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" ht="115.2">
       <c r="B5" s="67">
         <f t="shared" ref="B5:B12" si="0">C5+543</f>
         <v>2559</v>
@@ -14024,7 +14031,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="57" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" ht="57.6">
       <c r="B6" s="67">
         <f t="shared" si="0"/>
         <v>2560</v>
@@ -14037,7 +14044,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" ht="43.2">
       <c r="B7" s="67">
         <f t="shared" si="0"/>
         <v>2561</v>
@@ -14052,7 +14059,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="215.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" ht="215.4" customHeight="1">
       <c r="B8" s="67">
         <f t="shared" si="0"/>
         <v>2562</v>
@@ -14067,7 +14074,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="327.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" ht="345.6">
       <c r="B9" s="67">
         <f t="shared" si="0"/>
         <v>2563</v>
@@ -14082,7 +14089,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" ht="409.6">
       <c r="B10" s="67">
         <f t="shared" si="0"/>
         <v>2564</v>
@@ -14100,7 +14107,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" ht="409.6">
       <c r="B11" s="67">
         <f t="shared" si="0"/>
         <v>2565</v>
@@ -14118,7 +14125,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" ht="158.4">
       <c r="B12" s="67">
         <f t="shared" si="0"/>
         <v>2566</v>
@@ -14147,28 +14154,28 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="7.5" style="74" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="74" customWidth="1"/>
     <col min="3" max="3" width="94" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3">
       <c r="B1" s="74" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3">
       <c r="B2" s="74" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3">
       <c r="B3" s="74" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3">
       <c r="B4" s="74">
         <v>2018</v>
       </c>
@@ -14176,7 +14183,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="B5" s="74">
         <v>2019</v>
       </c>
@@ -14184,22 +14191,22 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3">
       <c r="C6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3">
       <c r="C7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3">
       <c r="B10" s="74" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3">
       <c r="B18" s="74" t="s">
         <v>114</v>
       </c>
@@ -14207,17 +14214,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3">
       <c r="B22" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3">
       <c r="B23" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3">
       <c r="B24" s="1" t="s">
         <v>123</v>
       </c>
@@ -14225,74 +14232,74 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3">
       <c r="B25" s="74" t="s">
         <v>124</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3">
       <c r="C26" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3">
       <c r="C27" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3">
       <c r="B28" s="74" t="s">
         <v>125</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3">
       <c r="C29" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3">
       <c r="C30" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3">
       <c r="C31" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3">
       <c r="B32" s="74" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3">
       <c r="C33" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3">
       <c r="B34" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3">
       <c r="C35" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3">
       <c r="B36" s="74" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3">
       <c r="C37" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3">
       <c r="C38" t="s">
         <v>133</v>
       </c>

</xml_diff>